<commit_message>
pasando todo a pyqt5
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -1,198 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chenaob\Documents\frisby\pdf\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD485CC-CD1C-4F82-9726-301152F289EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="MODELO" sheetId="1" r:id="rId1"/>
+    <sheet name="MODELO" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
-  <si>
-    <t>ENERGIA ELECTRICA</t>
-  </si>
-  <si>
-    <t>PER.DE COBRO</t>
-  </si>
-  <si>
-    <t>INFORMACIÓN CONTABILIDAD</t>
-  </si>
-  <si>
-    <t>INFORMACIÓN PPTOS</t>
-  </si>
-  <si>
-    <t>INICIAL</t>
-  </si>
-  <si>
-    <t>FINAL</t>
-  </si>
-  <si>
-    <t>CAUSA</t>
-  </si>
-  <si>
-    <t>PAGA</t>
-  </si>
-  <si>
-    <t>AJUS</t>
-  </si>
-  <si>
-    <t>DOC PAG</t>
-  </si>
-  <si>
-    <t>DOC AJ</t>
-  </si>
-  <si>
-    <t>CONSU ACT</t>
-  </si>
-  <si>
-    <t>CONSU REAC</t>
-  </si>
-  <si>
-    <t>KW</t>
-  </si>
-  <si>
-    <t>Vr  KW</t>
-  </si>
-  <si>
-    <t>Otros</t>
-  </si>
-  <si>
-    <t>ALUMBRADO</t>
-  </si>
-  <si>
-    <t>SERVICIO</t>
-  </si>
-  <si>
-    <t>EMPRESA</t>
-  </si>
-  <si>
-    <t>NIT</t>
-  </si>
-  <si>
-    <t>MEDIDOR</t>
-  </si>
-  <si>
-    <t>DIRECCION</t>
-  </si>
-  <si>
-    <t>ENERGIA</t>
-  </si>
-  <si>
-    <t>ELECTRICARIBE</t>
-  </si>
-  <si>
-    <t>802007670/911</t>
-  </si>
-  <si>
-    <t>CC. PLAZA BOCAGRANDE LOCAL 3-11</t>
-  </si>
-  <si>
-    <t>CR 1 12-120 ENTR BG1 LOC 311</t>
-  </si>
-  <si>
-    <t>PLAZA BOCAGRANDE CENTRO COMERCIAL</t>
-  </si>
-  <si>
-    <t>900785012/911</t>
-  </si>
-  <si>
-    <t>NIC 7742846</t>
-  </si>
-  <si>
-    <t>DEPOSITO 2 Y 4</t>
-  </si>
-  <si>
-    <t>CARIBERMAR DEL CARIBE</t>
-  </si>
-  <si>
-    <t>901380949/911</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="9">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
       <sz val="10"/>
-      <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
       <name val="Gill Sans"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="14"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="14"/>
       <name val="Gill Sans"/>
       <family val="2"/>
+      <b val="1"/>
+      <i val="1"/>
+      <sz val="14"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
       <name val="Gill Sans"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="9"/>
     </font>
     <font>
+      <name val="Gill Sans"/>
       <sz val="10"/>
-      <name val="Gill Sans"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
       <name val="Gill Sans"/>
       <family val="2"/>
+      <b val="1"/>
+      <color indexed="8"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
       <name val="Gill Sans"/>
       <family val="2"/>
+      <color indexed="8"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Gill Sans"/>
       <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -210,7 +91,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -838,137 +719,216 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="74">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="2" fillId="2" fontId="3" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="2" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="3" fillId="2" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="4" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="4" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="4" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="4" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="9" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="10" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="11" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="12" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="13" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="14" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="15" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="16" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="17" fillId="0" fontId="4" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="18" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="19" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="20" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="21" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="22" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="23" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="24" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="25" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="26" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="27" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="28" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="23" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="29" fillId="0" fontId="5" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="29" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="31" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="35" fillId="0" fontId="4" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="32" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="33" fillId="0" fontId="4" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="30" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="34" fillId="0" fontId="4" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="31" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="36" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="37" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="38" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="37" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="39" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="36" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="38" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="40" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="40" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="41" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="38" fillId="3" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="38" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="41" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="38" fillId="3" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="42" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="43" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="42" fillId="3" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="3" borderId="43" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="43" fillId="3" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="44" fillId="3" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="42" fillId="3" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="43" fillId="3" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="42" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="43" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="43" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="44" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="46" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="46" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="46" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="46" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="46" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="45" fillId="2" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 5" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal 5" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1292,8 +1252,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
@@ -1301,463 +1265,531 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="68" width="2.5703125"/>
+    <col customWidth="1" max="2" min="2" style="68" width="12.140625"/>
+    <col customWidth="1" max="3" min="3" style="68" width="12.7109375"/>
+    <col customWidth="1" max="4" min="4" style="68" width="14.140625"/>
+    <col customWidth="1" max="5" min="5" style="68" width="13.5703125"/>
+    <col customWidth="1" max="6" min="6" style="68" width="13.42578125"/>
+    <col customWidth="1" max="7" min="7" style="68" width="13.28515625"/>
+    <col customWidth="1" max="8" min="8" style="68" width="13"/>
+    <col customWidth="1" max="10" min="9" style="68" width="15.28515625"/>
+    <col customWidth="1" max="11" min="11" style="68" width="14.28515625"/>
+    <col customWidth="1" max="12" min="12" style="68" width="15.28515625"/>
+    <col customWidth="1" max="13" min="13" style="68" width="13.7109375"/>
+    <col customWidth="1" max="14" min="14" style="68" width="14.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="2" spans="1:14" ht="19.5" customHeight="1" thickBot="1">
-      <c r="B2" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="40"/>
-      <c r="I2" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="43"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B3" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="46">
+    <row customHeight="1" ht="15.75" r="1" s="68" thickBot="1"/>
+    <row customHeight="1" ht="19.5" r="2" s="68" thickBot="1">
+      <c r="B2" s="39" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="C2" s="40" t="n"/>
+      <c r="D2" s="41" t="inlineStr">
+        <is>
+          <t>EMPRESA</t>
+        </is>
+      </c>
+      <c r="E2" s="42" t="n"/>
+      <c r="F2" s="43" t="n"/>
+      <c r="G2" s="41" t="inlineStr">
+        <is>
+          <t>NIT</t>
+        </is>
+      </c>
+      <c r="H2" s="40" t="n"/>
+      <c r="I2" s="39" t="inlineStr">
+        <is>
+          <t>MEDIDOR</t>
+        </is>
+      </c>
+      <c r="J2" s="41" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="K2" s="40" t="n"/>
+      <c r="L2" s="40" t="n"/>
+      <c r="M2" s="40" t="n"/>
+      <c r="N2" s="43" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="3" s="68">
+      <c r="B3" s="44" t="inlineStr">
+        <is>
+          <t>ENERGIA</t>
+        </is>
+      </c>
+      <c r="C3" s="45" t="n"/>
+      <c r="D3" s="46" t="inlineStr">
+        <is>
+          <t>ELECTRICARIBE</t>
+        </is>
+      </c>
+      <c r="E3" s="47" t="n"/>
+      <c r="F3" s="48" t="n"/>
+      <c r="G3" s="46" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H3" s="45" t="n"/>
+      <c r="I3" s="46" t="n">
         <v>25782236</v>
       </c>
-      <c r="J3" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="48"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B4" s="50"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="52"/>
-      <c r="I4" s="54">
+      <c r="J3" s="49" t="inlineStr">
+        <is>
+          <t>CC. PLAZA BOCAGRANDE LOCAL 3-11</t>
+        </is>
+      </c>
+      <c r="K3" s="45" t="n"/>
+      <c r="L3" s="45" t="n"/>
+      <c r="M3" s="45" t="n"/>
+      <c r="N3" s="48" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" s="68">
+      <c r="B4" s="50" t="n"/>
+      <c r="C4" s="51" t="n"/>
+      <c r="D4" s="50" t="n"/>
+      <c r="E4" s="52" t="n"/>
+      <c r="F4" s="53" t="n"/>
+      <c r="G4" s="50" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H4" s="52" t="n"/>
+      <c r="I4" s="54" t="n">
         <v>25942309</v>
       </c>
-      <c r="J4" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="56"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B5" s="55"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="52"/>
-      <c r="I5" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="50"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="56"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B6" s="55"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="52"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="56"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B7" s="58"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="60" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="61"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="64"/>
-      <c r="I7" s="58" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="65"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="67"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A8" s="68"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="68"/>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B9" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B10" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="34"/>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B11" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B12" s="19"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="10"/>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B13" s="21"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="12"/>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B14" s="21"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="12"/>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B15" s="21"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="12"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1">
-      <c r="B16" s="21"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="12"/>
-    </row>
-    <row r="17" spans="2:14" ht="15.75" customHeight="1">
-      <c r="B17" s="21"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="12"/>
-    </row>
-    <row r="18" spans="2:14" ht="15.75" customHeight="1">
-      <c r="B18" s="21"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="12"/>
-    </row>
-    <row r="19" spans="2:14" ht="15.75" customHeight="1">
-      <c r="B19" s="21"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="12"/>
-    </row>
-    <row r="20" spans="2:14">
-      <c r="B20" s="21"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="12"/>
-    </row>
-    <row r="21" spans="2:14">
-      <c r="B21" s="21"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="12"/>
-    </row>
-    <row r="22" spans="2:14">
-      <c r="B22" s="21"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="12"/>
-    </row>
-    <row r="23" spans="2:14">
-      <c r="B23" s="21"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="12"/>
-    </row>
-    <row r="24" spans="2:14">
-      <c r="B24" s="21"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="12"/>
-    </row>
-    <row r="25" spans="2:14" ht="15.75" thickBot="1">
-      <c r="B25" s="23"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="14"/>
+      <c r="J4" s="55" t="inlineStr">
+        <is>
+          <t>CR 1 12-120 ENTR BG1 LOC 311</t>
+        </is>
+      </c>
+      <c r="K4" s="52" t="n"/>
+      <c r="L4" s="52" t="n"/>
+      <c r="M4" s="52" t="n"/>
+      <c r="N4" s="56" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" s="68">
+      <c r="B5" s="55" t="n"/>
+      <c r="C5" s="51" t="n"/>
+      <c r="D5" s="50" t="inlineStr">
+        <is>
+          <t>PLAZA BOCAGRANDE CENTRO COMERCIAL</t>
+        </is>
+      </c>
+      <c r="E5" s="51" t="n"/>
+      <c r="F5" s="53" t="n"/>
+      <c r="G5" s="50" t="inlineStr">
+        <is>
+          <t>900785012/911</t>
+        </is>
+      </c>
+      <c r="H5" s="52" t="n"/>
+      <c r="I5" s="57" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J5" s="50" t="n"/>
+      <c r="K5" s="52" t="n"/>
+      <c r="L5" s="52" t="n"/>
+      <c r="M5" s="52" t="n"/>
+      <c r="N5" s="56" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" s="68">
+      <c r="B6" s="55" t="n"/>
+      <c r="C6" s="51" t="n"/>
+      <c r="D6" s="55" t="n"/>
+      <c r="E6" s="51" t="n"/>
+      <c r="F6" s="53" t="n"/>
+      <c r="G6" s="46" t="inlineStr">
+        <is>
+          <t>DEPOSITO 2 Y 4</t>
+        </is>
+      </c>
+      <c r="H6" s="52" t="n"/>
+      <c r="I6" s="55" t="n"/>
+      <c r="J6" s="50" t="n"/>
+      <c r="K6" s="52" t="n"/>
+      <c r="L6" s="52" t="n"/>
+      <c r="M6" s="52" t="n"/>
+      <c r="N6" s="56" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="68" thickBot="1">
+      <c r="B7" s="58" t="n"/>
+      <c r="C7" s="59" t="n"/>
+      <c r="D7" s="60" t="inlineStr">
+        <is>
+          <t>CARIBERMAR DEL CARIBE</t>
+        </is>
+      </c>
+      <c r="E7" s="61" t="n"/>
+      <c r="F7" s="62" t="n"/>
+      <c r="G7" s="63" t="inlineStr">
+        <is>
+          <t>901380949/911</t>
+        </is>
+      </c>
+      <c r="H7" s="64" t="n"/>
+      <c r="I7" s="58" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J7" s="65" t="n"/>
+      <c r="K7" s="66" t="n"/>
+      <c r="L7" s="59" t="n"/>
+      <c r="M7" s="59" t="n"/>
+      <c r="N7" s="67" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="8" s="68" thickBot="1">
+      <c r="B8" s="69" t="n"/>
+      <c r="C8" s="69" t="n"/>
+      <c r="D8" s="70" t="n"/>
+      <c r="E8" s="69" t="n"/>
+      <c r="F8" s="69" t="n"/>
+      <c r="G8" s="69" t="n"/>
+      <c r="H8" s="71" t="n"/>
+      <c r="I8" s="69" t="n"/>
+      <c r="J8" s="71" t="n"/>
+      <c r="K8" s="71" t="n"/>
+      <c r="L8" s="69" t="n"/>
+      <c r="M8" s="72" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="9" s="68" thickBot="1">
+      <c r="B9" s="73" t="inlineStr">
+        <is>
+          <t>ENERGIA ELECTRICA</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+      <c r="E9" s="1" t="n"/>
+      <c r="F9" s="1" t="n"/>
+      <c r="G9" s="1" t="n"/>
+      <c r="H9" s="1" t="n"/>
+      <c r="I9" s="2" t="n"/>
+      <c r="J9" s="2" t="n"/>
+      <c r="K9" s="2" t="n"/>
+      <c r="L9" s="2" t="n"/>
+      <c r="M9" s="2" t="n"/>
+      <c r="N9" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" s="68" thickBot="1">
+      <c r="B10" s="35" t="inlineStr">
+        <is>
+          <t>PER.DE COBRO</t>
+        </is>
+      </c>
+      <c r="C10" s="36" t="n"/>
+      <c r="D10" s="37" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="E10" s="38" t="n"/>
+      <c r="F10" s="38" t="n"/>
+      <c r="G10" s="38" t="n"/>
+      <c r="H10" s="36" t="n"/>
+      <c r="I10" s="33" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN PPTOS</t>
+        </is>
+      </c>
+      <c r="J10" s="38" t="n"/>
+      <c r="K10" s="38" t="n"/>
+      <c r="L10" s="38" t="n"/>
+      <c r="M10" s="38" t="n"/>
+      <c r="N10" s="34" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="11" s="68" thickBot="1">
+      <c r="B11" s="17" t="inlineStr">
+        <is>
+          <t>INICIAL</t>
+        </is>
+      </c>
+      <c r="C11" s="6" t="inlineStr">
+        <is>
+          <t>FINAL</t>
+        </is>
+      </c>
+      <c r="D11" s="6" t="inlineStr">
+        <is>
+          <t>CAUSA</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="inlineStr">
+        <is>
+          <t>PAGA</t>
+        </is>
+      </c>
+      <c r="F11" s="6" t="inlineStr">
+        <is>
+          <t>AJUS</t>
+        </is>
+      </c>
+      <c r="G11" s="6" t="inlineStr">
+        <is>
+          <t>DOC PAG</t>
+        </is>
+      </c>
+      <c r="H11" s="6" t="inlineStr">
+        <is>
+          <t>DOC AJ</t>
+        </is>
+      </c>
+      <c r="I11" s="4" t="inlineStr">
+        <is>
+          <t>CONSU ACT</t>
+        </is>
+      </c>
+      <c r="J11" s="5" t="inlineStr">
+        <is>
+          <t>CONSU REAC</t>
+        </is>
+      </c>
+      <c r="K11" s="5" t="inlineStr">
+        <is>
+          <t>KW</t>
+        </is>
+      </c>
+      <c r="L11" s="5" t="inlineStr">
+        <is>
+          <t>Vr  KW</t>
+        </is>
+      </c>
+      <c r="M11" s="6" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="N11" s="7" t="inlineStr">
+        <is>
+          <t>ALUMBRADO</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="12" s="68">
+      <c r="B12" s="19" t="n"/>
+      <c r="C12" s="25" t="n"/>
+      <c r="D12" s="19" t="n"/>
+      <c r="E12" s="28" t="n"/>
+      <c r="F12" s="28" t="n"/>
+      <c r="G12" s="28" t="n"/>
+      <c r="H12" s="20" t="n"/>
+      <c r="I12" s="8" t="n"/>
+      <c r="J12" s="8" t="n"/>
+      <c r="K12" s="9" t="n"/>
+      <c r="L12" s="9" t="n"/>
+      <c r="M12" s="9" t="n"/>
+      <c r="N12" s="10" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="13" s="68">
+      <c r="B13" s="21" t="n"/>
+      <c r="C13" s="26" t="n"/>
+      <c r="D13" s="21" t="n"/>
+      <c r="E13" s="18" t="n"/>
+      <c r="F13" s="18" t="n"/>
+      <c r="G13" s="18" t="n"/>
+      <c r="H13" s="22" t="n"/>
+      <c r="I13" s="15" t="n"/>
+      <c r="J13" s="15" t="n"/>
+      <c r="K13" s="11" t="n"/>
+      <c r="L13" s="11" t="n"/>
+      <c r="M13" s="11" t="n"/>
+      <c r="N13" s="12" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="14" s="68">
+      <c r="B14" s="21" t="n"/>
+      <c r="C14" s="26" t="n"/>
+      <c r="D14" s="21" t="n"/>
+      <c r="E14" s="18" t="n"/>
+      <c r="F14" s="18" t="n"/>
+      <c r="G14" s="18" t="n"/>
+      <c r="H14" s="22" t="n"/>
+      <c r="I14" s="15" t="n"/>
+      <c r="J14" s="15" t="n"/>
+      <c r="K14" s="11" t="n"/>
+      <c r="L14" s="11" t="n"/>
+      <c r="M14" s="11" t="n"/>
+      <c r="N14" s="12" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" s="68">
+      <c r="B15" s="21" t="n"/>
+      <c r="C15" s="26" t="n"/>
+      <c r="D15" s="21" t="n"/>
+      <c r="E15" s="18" t="n"/>
+      <c r="F15" s="18" t="n"/>
+      <c r="G15" s="18" t="n"/>
+      <c r="H15" s="22" t="n"/>
+      <c r="I15" s="15" t="n"/>
+      <c r="J15" s="15" t="n"/>
+      <c r="K15" s="11" t="n"/>
+      <c r="L15" s="11" t="n"/>
+      <c r="M15" s="11" t="n"/>
+      <c r="N15" s="12" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="16" s="68">
+      <c r="B16" s="21" t="n"/>
+      <c r="C16" s="26" t="n"/>
+      <c r="D16" s="21" t="n"/>
+      <c r="E16" s="18" t="n"/>
+      <c r="F16" s="18" t="n"/>
+      <c r="G16" s="18" t="n"/>
+      <c r="H16" s="22" t="n"/>
+      <c r="I16" s="15" t="n"/>
+      <c r="J16" s="15" t="n"/>
+      <c r="K16" s="11" t="n"/>
+      <c r="L16" s="11" t="n"/>
+      <c r="M16" s="11" t="n"/>
+      <c r="N16" s="12" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="17" s="68">
+      <c r="B17" s="21" t="n"/>
+      <c r="C17" s="26" t="n"/>
+      <c r="D17" s="21" t="n"/>
+      <c r="E17" s="18" t="n"/>
+      <c r="F17" s="18" t="n"/>
+      <c r="G17" s="18" t="n"/>
+      <c r="H17" s="22" t="n"/>
+      <c r="I17" s="15" t="n"/>
+      <c r="J17" s="15" t="n"/>
+      <c r="K17" s="11" t="n"/>
+      <c r="L17" s="11" t="n"/>
+      <c r="M17" s="11" t="n"/>
+      <c r="N17" s="12" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="18" s="68">
+      <c r="B18" s="21" t="n"/>
+      <c r="C18" s="26" t="n"/>
+      <c r="D18" s="21" t="n"/>
+      <c r="E18" s="18" t="n"/>
+      <c r="F18" s="18" t="n"/>
+      <c r="G18" s="18" t="n"/>
+      <c r="H18" s="22" t="n"/>
+      <c r="I18" s="15" t="n"/>
+      <c r="J18" s="15" t="n"/>
+      <c r="K18" s="11" t="n"/>
+      <c r="L18" s="11" t="n"/>
+      <c r="M18" s="11" t="n"/>
+      <c r="N18" s="12" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" s="68">
+      <c r="B19" s="21" t="n"/>
+      <c r="C19" s="26" t="n"/>
+      <c r="D19" s="21" t="n"/>
+      <c r="E19" s="18" t="n"/>
+      <c r="F19" s="18" t="n"/>
+      <c r="G19" s="18" t="n"/>
+      <c r="H19" s="22" t="n"/>
+      <c r="I19" s="15" t="n"/>
+      <c r="J19" s="15" t="n"/>
+      <c r="K19" s="11" t="n"/>
+      <c r="L19" s="11" t="n"/>
+      <c r="M19" s="11" t="n"/>
+      <c r="N19" s="12" t="n"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="21" t="n"/>
+      <c r="C20" s="26" t="n"/>
+      <c r="D20" s="21" t="n"/>
+      <c r="E20" s="18" t="n"/>
+      <c r="F20" s="18" t="n"/>
+      <c r="G20" s="18" t="n"/>
+      <c r="H20" s="22" t="n"/>
+      <c r="I20" s="15" t="n"/>
+      <c r="J20" s="15" t="n"/>
+      <c r="K20" s="11" t="n"/>
+      <c r="L20" s="11" t="n"/>
+      <c r="M20" s="11" t="n"/>
+      <c r="N20" s="12" t="n"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="21" t="n"/>
+      <c r="C21" s="26" t="n"/>
+      <c r="D21" s="21" t="n"/>
+      <c r="E21" s="18" t="n"/>
+      <c r="F21" s="18" t="n"/>
+      <c r="G21" s="18" t="n"/>
+      <c r="H21" s="22" t="n"/>
+      <c r="I21" s="15" t="n"/>
+      <c r="J21" s="15" t="n"/>
+      <c r="K21" s="11" t="n"/>
+      <c r="L21" s="11" t="n"/>
+      <c r="M21" s="11" t="n"/>
+      <c r="N21" s="12" t="n"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="21" t="n"/>
+      <c r="C22" s="26" t="n"/>
+      <c r="D22" s="21" t="n"/>
+      <c r="E22" s="18" t="n"/>
+      <c r="F22" s="18" t="n"/>
+      <c r="G22" s="18" t="n"/>
+      <c r="H22" s="22" t="n"/>
+      <c r="I22" s="15" t="n"/>
+      <c r="J22" s="15" t="n"/>
+      <c r="K22" s="11" t="n"/>
+      <c r="L22" s="11" t="n"/>
+      <c r="M22" s="11" t="n"/>
+      <c r="N22" s="12" t="n"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="21" t="n"/>
+      <c r="C23" s="26" t="n"/>
+      <c r="D23" s="21" t="n"/>
+      <c r="E23" s="18" t="n"/>
+      <c r="F23" s="18" t="n"/>
+      <c r="G23" s="18" t="n"/>
+      <c r="H23" s="22" t="n"/>
+      <c r="I23" s="15" t="n"/>
+      <c r="J23" s="15" t="n"/>
+      <c r="K23" s="11" t="n"/>
+      <c r="L23" s="11" t="n"/>
+      <c r="M23" s="11" t="n"/>
+      <c r="N23" s="12" t="n"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="21" t="n"/>
+      <c r="C24" s="26" t="n"/>
+      <c r="D24" s="21" t="n"/>
+      <c r="E24" s="18" t="n"/>
+      <c r="F24" s="18" t="n"/>
+      <c r="G24" s="18" t="n"/>
+      <c r="H24" s="22" t="n"/>
+      <c r="I24" s="15" t="n"/>
+      <c r="J24" s="15" t="n"/>
+      <c r="K24" s="11" t="n"/>
+      <c r="L24" s="11" t="n"/>
+      <c r="M24" s="11" t="n"/>
+      <c r="N24" s="12" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="25" s="68" thickBot="1">
+      <c r="B25" s="23" t="n"/>
+      <c r="C25" s="27" t="n"/>
+      <c r="D25" s="29" t="n"/>
+      <c r="E25" s="30" t="n"/>
+      <c r="F25" s="30" t="n"/>
+      <c r="G25" s="31" t="n"/>
+      <c r="H25" s="24" t="n"/>
+      <c r="I25" s="16" t="n"/>
+      <c r="J25" s="16" t="n"/>
+      <c r="K25" s="13" t="n"/>
+      <c r="L25" s="13" t="n"/>
+      <c r="M25" s="13" t="n"/>
+      <c r="N25" s="14" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:H10"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mas o menos todo bien falta poner causalidad automatica
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -9,6 +9,13 @@
   <sheets>
     <sheet name="MODELO" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="4" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="5" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="6" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="7" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="8" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
@@ -1525,92 +1532,3250 @@
     <row customHeight="1" ht="15.75" r="12" s="32">
       <c r="B12" s="56" t="inlineStr">
         <is>
-          <t>2020-09-11</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="C12" s="57" t="inlineStr">
         <is>
-          <t>2020-10-10</t>
+          <t>2020-10-06</t>
         </is>
       </c>
       <c r="D12" s="57" t="n">
-        <v>12000000</v>
+        <v>12333333</v>
       </c>
       <c r="E12" s="57" t="n">
-        <v>4760727</v>
+        <v>1491386</v>
       </c>
       <c r="F12" s="57" t="n">
-        <v>-7239273</v>
+        <v>-10841947</v>
       </c>
       <c r="G12" s="57" t="n">
-        <v>12</v>
+        <v>122</v>
       </c>
       <c r="H12" s="57" t="n">
         <v>12</v>
       </c>
       <c r="I12" s="57" t="n">
+        <v>1284935</v>
+      </c>
+      <c r="J12" s="57" t="n">
+        <v>80026</v>
+      </c>
+      <c r="K12" s="57" t="n">
+        <v>2131</v>
+      </c>
+      <c r="L12" s="57" t="n">
+        <v>602.9728</v>
+      </c>
+      <c r="M12" s="57" t="n">
+        <v>256987</v>
+      </c>
+      <c r="N12" s="58" t="n">
+        <v>58680</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="13" s="32">
+      <c r="B13" s="59" t="inlineStr">
+        <is>
+          <t>2020-09-11</t>
+        </is>
+      </c>
+      <c r="C13" s="31" t="inlineStr">
+        <is>
+          <t>2020-10-10</t>
+        </is>
+      </c>
+      <c r="D13" s="31" t="n">
+        <v>12000000</v>
+      </c>
+      <c r="E13" s="31" t="n">
+        <v>4760727</v>
+      </c>
+      <c r="F13" s="31" t="n">
+        <v>-7239273</v>
+      </c>
+      <c r="G13" s="31" t="n">
+        <v>12</v>
+      </c>
+      <c r="H13" s="31" t="n">
+        <v>12</v>
+      </c>
+      <c r="I13" s="31" t="n">
         <v>4530777</v>
+      </c>
+      <c r="J13" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="31" t="n">
+        <v>8040</v>
+      </c>
+      <c r="L13" s="31" t="n">
+        <v>563.5295</v>
+      </c>
+      <c r="M13" s="31" t="n">
+        <v>906155</v>
+      </c>
+      <c r="N13" s="60" t="n">
+        <v>197790</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="14" s="32">
+      <c r="B14" s="59" t="inlineStr">
+        <is>
+          <t>2020-09-11</t>
+        </is>
+      </c>
+      <c r="C14" s="31" t="inlineStr">
+        <is>
+          <t>2020-10-10</t>
+        </is>
+      </c>
+      <c r="D14" s="31" t="n">
+        <v>12000000</v>
+      </c>
+      <c r="E14" s="31" t="n">
+        <v>4760727</v>
+      </c>
+      <c r="F14" s="31" t="n">
+        <v>-7239273</v>
+      </c>
+      <c r="G14" s="31" t="n">
+        <v>45</v>
+      </c>
+      <c r="H14" s="31" t="n">
+        <v>45</v>
+      </c>
+      <c r="I14" s="31" t="n">
+        <v>4530777</v>
+      </c>
+      <c r="J14" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="31" t="n">
+        <v>8040</v>
+      </c>
+      <c r="L14" s="31" t="n">
+        <v>563.5295</v>
+      </c>
+      <c r="M14" s="31" t="n">
+        <v>906155</v>
+      </c>
+      <c r="N14" s="60" t="n">
+        <v>197790</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" s="32">
+      <c r="B15" s="59" t="n"/>
+      <c r="N15" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="16" s="32">
+      <c r="B16" s="59" t="n"/>
+      <c r="N16" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="17" s="32">
+      <c r="B17" s="59" t="n"/>
+      <c r="N17" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="18" s="32">
+      <c r="B18" s="59" t="n"/>
+      <c r="N18" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" s="32">
+      <c r="B19" s="59" t="n"/>
+      <c r="N19" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="20" s="32">
+      <c r="B20" s="59" t="n"/>
+      <c r="N20" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="21" s="32">
+      <c r="B21" s="59" t="n"/>
+      <c r="N21" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="22" s="32">
+      <c r="B22" s="59" t="n"/>
+      <c r="N22" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="23" s="32">
+      <c r="B23" s="59" t="n"/>
+      <c r="N23" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="24" s="32">
+      <c r="B24" s="61" t="n"/>
+      <c r="C24" s="62" t="n"/>
+      <c r="D24" s="62" t="n"/>
+      <c r="E24" s="62" t="n"/>
+      <c r="F24" s="62" t="n"/>
+      <c r="G24" s="62" t="n"/>
+      <c r="H24" s="62" t="n"/>
+      <c r="I24" s="62" t="n"/>
+      <c r="J24" s="62" t="n"/>
+      <c r="K24" s="62" t="n"/>
+      <c r="L24" s="62" t="n"/>
+      <c r="M24" s="62" t="n"/>
+      <c r="N24" s="63" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="25" s="32"/>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="B9:N9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="I10:N10"/>
+  </mergeCells>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="B2:O24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.18359375" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="31" width="2.57"/>
+    <col customWidth="1" max="2" min="2" style="31" width="12.14"/>
+    <col customWidth="1" max="3" min="3" style="31" width="12.71"/>
+    <col customWidth="1" max="4" min="4" style="31" width="14.15"/>
+    <col customWidth="1" max="5" min="5" style="31" width="13.57"/>
+    <col customWidth="1" max="6" min="6" style="31" width="13.43"/>
+    <col customWidth="1" max="7" min="7" style="31" width="13.29"/>
+    <col customWidth="1" max="8" min="8" style="31" width="13.02"/>
+    <col customWidth="1" max="10" min="9" style="31" width="15.29"/>
+    <col customWidth="1" max="11" min="11" style="31" width="14.28"/>
+    <col customWidth="1" max="12" min="12" style="31" width="15.29"/>
+    <col customWidth="1" max="13" min="13" style="31" width="13.7"/>
+    <col customWidth="1" max="14" min="14" style="31" width="14.15"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15.75" r="1" s="32"/>
+    <row customHeight="1" ht="19.5" r="2" s="32">
+      <c r="B2" s="33" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="C2" s="34" t="n"/>
+      <c r="D2" s="35" t="inlineStr">
+        <is>
+          <t>EMPRESA</t>
+        </is>
+      </c>
+      <c r="E2" s="34" t="n"/>
+      <c r="F2" s="34" t="n"/>
+      <c r="G2" s="35" t="inlineStr">
+        <is>
+          <t>NIT</t>
+        </is>
+      </c>
+      <c r="H2" s="34" t="n"/>
+      <c r="I2" s="36" t="inlineStr">
+        <is>
+          <t>MEDIDOR</t>
+        </is>
+      </c>
+      <c r="J2" s="37" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="K2" s="34" t="n"/>
+      <c r="L2" s="34" t="n"/>
+      <c r="M2" s="34" t="n"/>
+      <c r="N2" s="38" t="n"/>
+      <c r="O2" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="3" s="32">
+      <c r="B3" s="40" t="inlineStr">
+        <is>
+          <t>ENERGIA</t>
+        </is>
+      </c>
+      <c r="C3" s="34" t="n"/>
+      <c r="D3" s="41" t="inlineStr">
+        <is>
+          <t>ELECTRICARIBE</t>
+        </is>
+      </c>
+      <c r="E3" s="34" t="n"/>
+      <c r="F3" s="34" t="n"/>
+      <c r="G3" s="41" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H3" s="34" t="n"/>
+      <c r="I3" s="42" t="n">
+        <v>25782236</v>
+      </c>
+      <c r="J3" s="43" t="inlineStr">
+        <is>
+          <t>CC. PLAZA BOCAGRANDE LOCAL 3-11</t>
+        </is>
+      </c>
+      <c r="K3" s="34" t="n"/>
+      <c r="L3" s="34" t="n"/>
+      <c r="M3" s="34" t="n"/>
+      <c r="N3" s="38" t="n"/>
+      <c r="O3" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" s="32">
+      <c r="B4" s="40" t="n"/>
+      <c r="C4" s="34" t="n"/>
+      <c r="D4" s="40" t="n"/>
+      <c r="E4" s="34" t="n"/>
+      <c r="F4" s="34" t="n"/>
+      <c r="G4" s="40" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H4" s="34" t="n"/>
+      <c r="I4" s="44" t="n">
+        <v>25942309</v>
+      </c>
+      <c r="J4" s="43" t="inlineStr">
+        <is>
+          <t>CR 1 12-120 ENTR BG1 LOC 311</t>
+        </is>
+      </c>
+      <c r="K4" s="34" t="n"/>
+      <c r="L4" s="34" t="n"/>
+      <c r="M4" s="34" t="n"/>
+      <c r="N4" s="38" t="n"/>
+      <c r="O4" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" s="32">
+      <c r="B5" s="45" t="n"/>
+      <c r="C5" s="34" t="n"/>
+      <c r="D5" s="40" t="inlineStr">
+        <is>
+          <t>PLAZA BOCAGRANDE CENTRO COMERCIAL</t>
+        </is>
+      </c>
+      <c r="E5" s="34" t="n"/>
+      <c r="F5" s="34" t="n"/>
+      <c r="G5" s="40" t="inlineStr">
+        <is>
+          <t>900785012/911</t>
+        </is>
+      </c>
+      <c r="H5" s="34" t="n"/>
+      <c r="I5" s="46" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J5" s="47" t="n"/>
+      <c r="K5" s="34" t="n"/>
+      <c r="L5" s="34" t="n"/>
+      <c r="M5" s="34" t="n"/>
+      <c r="N5" s="38" t="n"/>
+      <c r="O5" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" s="32">
+      <c r="B6" s="45" t="n"/>
+      <c r="C6" s="34" t="n"/>
+      <c r="D6" s="45" t="n"/>
+      <c r="E6" s="34" t="n"/>
+      <c r="F6" s="34" t="n"/>
+      <c r="G6" s="41" t="inlineStr">
+        <is>
+          <t>DEPOSITO 2 Y 4</t>
+        </is>
+      </c>
+      <c r="H6" s="34" t="n"/>
+      <c r="I6" s="48" t="n"/>
+      <c r="J6" s="47" t="n"/>
+      <c r="K6" s="34" t="n"/>
+      <c r="L6" s="34" t="n"/>
+      <c r="M6" s="34" t="n"/>
+      <c r="N6" s="38" t="n"/>
+      <c r="O6" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="32">
+      <c r="B7" s="45" t="n"/>
+      <c r="C7" s="34" t="n"/>
+      <c r="D7" s="49" t="inlineStr">
+        <is>
+          <t>CARIBERMAR DEL CARIBE</t>
+        </is>
+      </c>
+      <c r="E7" s="34" t="n"/>
+      <c r="F7" s="34" t="n"/>
+      <c r="G7" s="49" t="inlineStr">
+        <is>
+          <t>901380949/911</t>
+        </is>
+      </c>
+      <c r="H7" s="34" t="n"/>
+      <c r="I7" s="48" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J7" s="43" t="n"/>
+      <c r="K7" s="34" t="n"/>
+      <c r="L7" s="34" t="n"/>
+      <c r="M7" s="34" t="n"/>
+      <c r="N7" s="38" t="n"/>
+      <c r="O7" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="8" s="32">
+      <c r="B8" s="50" t="n"/>
+      <c r="C8" s="50" t="n"/>
+      <c r="D8" s="51" t="n"/>
+      <c r="E8" s="50" t="n"/>
+      <c r="F8" s="50" t="n"/>
+      <c r="G8" s="50" t="n"/>
+      <c r="H8" s="51" t="n"/>
+      <c r="I8" s="50" t="n"/>
+      <c r="J8" s="51" t="n"/>
+      <c r="K8" s="51" t="n"/>
+      <c r="L8" s="50" t="n"/>
+      <c r="M8" s="52" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="9" s="32">
+      <c r="B9" s="53" t="inlineStr">
+        <is>
+          <t>ENERGIA ELECTRICA</t>
+        </is>
+      </c>
+      <c r="C9" s="34" t="n"/>
+      <c r="D9" s="34" t="n"/>
+      <c r="E9" s="34" t="n"/>
+      <c r="F9" s="34" t="n"/>
+      <c r="G9" s="34" t="n"/>
+      <c r="H9" s="34" t="n"/>
+      <c r="I9" s="34" t="n"/>
+      <c r="J9" s="34" t="n"/>
+      <c r="K9" s="34" t="n"/>
+      <c r="L9" s="34" t="n"/>
+      <c r="M9" s="34" t="n"/>
+      <c r="N9" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" s="32">
+      <c r="B10" s="54" t="inlineStr">
+        <is>
+          <t>PER.DE COBRO</t>
+        </is>
+      </c>
+      <c r="C10" s="38" t="n"/>
+      <c r="D10" s="54" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="E10" s="34" t="n"/>
+      <c r="F10" s="34" t="n"/>
+      <c r="G10" s="34" t="n"/>
+      <c r="H10" s="38" t="n"/>
+      <c r="I10" s="55" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN PPTOS</t>
+        </is>
+      </c>
+      <c r="J10" s="34" t="n"/>
+      <c r="K10" s="34" t="n"/>
+      <c r="L10" s="34" t="n"/>
+      <c r="M10" s="34" t="n"/>
+      <c r="N10" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="11" s="32">
+      <c r="B11" s="54" t="inlineStr">
+        <is>
+          <t>INICIAL</t>
+        </is>
+      </c>
+      <c r="C11" s="54" t="inlineStr">
+        <is>
+          <t>FINAL</t>
+        </is>
+      </c>
+      <c r="D11" s="54" t="inlineStr">
+        <is>
+          <t>CAUSA</t>
+        </is>
+      </c>
+      <c r="E11" s="54" t="inlineStr">
+        <is>
+          <t>PAGA</t>
+        </is>
+      </c>
+      <c r="F11" s="54" t="inlineStr">
+        <is>
+          <t>AJUS</t>
+        </is>
+      </c>
+      <c r="G11" s="54" t="inlineStr">
+        <is>
+          <t>DOC PAG</t>
+        </is>
+      </c>
+      <c r="H11" s="54" t="inlineStr">
+        <is>
+          <t>DOC AJ</t>
+        </is>
+      </c>
+      <c r="I11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU ACT</t>
+        </is>
+      </c>
+      <c r="J11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU REAC</t>
+        </is>
+      </c>
+      <c r="K11" s="54" t="inlineStr">
+        <is>
+          <t>KW</t>
+        </is>
+      </c>
+      <c r="L11" s="54" t="inlineStr">
+        <is>
+          <t>Vr  KW</t>
+        </is>
+      </c>
+      <c r="M11" s="54" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="N11" s="54" t="inlineStr">
+        <is>
+          <t>ALUMBRADO</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="12" s="32">
+      <c r="B12" s="56" t="n"/>
+      <c r="C12" s="57" t="n"/>
+      <c r="D12" s="57" t="n"/>
+      <c r="E12" s="57" t="n"/>
+      <c r="F12" s="57" t="n"/>
+      <c r="G12" s="57" t="n"/>
+      <c r="H12" s="57" t="n"/>
+      <c r="I12" s="57" t="n"/>
+      <c r="J12" s="57" t="n"/>
+      <c r="K12" s="57" t="n"/>
+      <c r="L12" s="57" t="n"/>
+      <c r="M12" s="57" t="n"/>
+      <c r="N12" s="58" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="13" s="32">
+      <c r="B13" s="59" t="n"/>
+      <c r="N13" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="14" s="32">
+      <c r="B14" s="59" t="n"/>
+      <c r="N14" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" s="32">
+      <c r="B15" s="59" t="n"/>
+      <c r="N15" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="16" s="32">
+      <c r="B16" s="59" t="n"/>
+      <c r="N16" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="17" s="32">
+      <c r="B17" s="59" t="n"/>
+      <c r="N17" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="18" s="32">
+      <c r="B18" s="59" t="n"/>
+      <c r="N18" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" s="32">
+      <c r="B19" s="59" t="n"/>
+      <c r="N19" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="20" s="32">
+      <c r="B20" s="59" t="n"/>
+      <c r="N20" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="21" s="32">
+      <c r="B21" s="59" t="n"/>
+      <c r="N21" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="22" s="32">
+      <c r="B22" s="59" t="n"/>
+      <c r="N22" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="23" s="32">
+      <c r="B23" s="59" t="n"/>
+      <c r="N23" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="24" s="32">
+      <c r="B24" s="61" t="n"/>
+      <c r="C24" s="62" t="n"/>
+      <c r="D24" s="62" t="n"/>
+      <c r="E24" s="62" t="n"/>
+      <c r="F24" s="62" t="n"/>
+      <c r="G24" s="62" t="n"/>
+      <c r="H24" s="62" t="n"/>
+      <c r="I24" s="62" t="n"/>
+      <c r="J24" s="62" t="n"/>
+      <c r="K24" s="62" t="n"/>
+      <c r="L24" s="62" t="n"/>
+      <c r="M24" s="62" t="n"/>
+      <c r="N24" s="63" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="25" s="32"/>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="B9:N9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="I10:N10"/>
+  </mergeCells>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="B2:O24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.18359375" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="31" width="2.57"/>
+    <col customWidth="1" max="2" min="2" style="31" width="12.14"/>
+    <col customWidth="1" max="3" min="3" style="31" width="12.71"/>
+    <col customWidth="1" max="4" min="4" style="31" width="14.15"/>
+    <col customWidth="1" max="5" min="5" style="31" width="13.57"/>
+    <col customWidth="1" max="6" min="6" style="31" width="13.43"/>
+    <col customWidth="1" max="7" min="7" style="31" width="13.29"/>
+    <col customWidth="1" max="8" min="8" style="31" width="13.02"/>
+    <col customWidth="1" max="10" min="9" style="31" width="15.29"/>
+    <col customWidth="1" max="11" min="11" style="31" width="14.28"/>
+    <col customWidth="1" max="12" min="12" style="31" width="15.29"/>
+    <col customWidth="1" max="13" min="13" style="31" width="13.7"/>
+    <col customWidth="1" max="14" min="14" style="31" width="14.15"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15.75" r="1" s="32"/>
+    <row customHeight="1" ht="19.5" r="2" s="32">
+      <c r="B2" s="33" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="C2" s="34" t="n"/>
+      <c r="D2" s="35" t="inlineStr">
+        <is>
+          <t>EMPRESA</t>
+        </is>
+      </c>
+      <c r="E2" s="34" t="n"/>
+      <c r="F2" s="34" t="n"/>
+      <c r="G2" s="35" t="inlineStr">
+        <is>
+          <t>NIT</t>
+        </is>
+      </c>
+      <c r="H2" s="34" t="n"/>
+      <c r="I2" s="36" t="inlineStr">
+        <is>
+          <t>MEDIDOR</t>
+        </is>
+      </c>
+      <c r="J2" s="37" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="K2" s="34" t="n"/>
+      <c r="L2" s="34" t="n"/>
+      <c r="M2" s="34" t="n"/>
+      <c r="N2" s="38" t="n"/>
+      <c r="O2" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="3" s="32">
+      <c r="B3" s="40" t="inlineStr">
+        <is>
+          <t>ENERGIA</t>
+        </is>
+      </c>
+      <c r="C3" s="34" t="n"/>
+      <c r="D3" s="41" t="inlineStr">
+        <is>
+          <t>ELECTRICARIBE</t>
+        </is>
+      </c>
+      <c r="E3" s="34" t="n"/>
+      <c r="F3" s="34" t="n"/>
+      <c r="G3" s="41" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H3" s="34" t="n"/>
+      <c r="I3" s="42" t="n">
+        <v>25782236</v>
+      </c>
+      <c r="J3" s="43" t="inlineStr">
+        <is>
+          <t>CC. PLAZA BOCAGRANDE LOCAL 3-11</t>
+        </is>
+      </c>
+      <c r="K3" s="34" t="n"/>
+      <c r="L3" s="34" t="n"/>
+      <c r="M3" s="34" t="n"/>
+      <c r="N3" s="38" t="n"/>
+      <c r="O3" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" s="32">
+      <c r="B4" s="40" t="n"/>
+      <c r="C4" s="34" t="n"/>
+      <c r="D4" s="40" t="n"/>
+      <c r="E4" s="34" t="n"/>
+      <c r="F4" s="34" t="n"/>
+      <c r="G4" s="40" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H4" s="34" t="n"/>
+      <c r="I4" s="44" t="n">
+        <v>25942309</v>
+      </c>
+      <c r="J4" s="43" t="inlineStr">
+        <is>
+          <t>CR 1 12-120 ENTR BG1 LOC 311</t>
+        </is>
+      </c>
+      <c r="K4" s="34" t="n"/>
+      <c r="L4" s="34" t="n"/>
+      <c r="M4" s="34" t="n"/>
+      <c r="N4" s="38" t="n"/>
+      <c r="O4" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" s="32">
+      <c r="B5" s="45" t="n"/>
+      <c r="C5" s="34" t="n"/>
+      <c r="D5" s="40" t="inlineStr">
+        <is>
+          <t>PLAZA BOCAGRANDE CENTRO COMERCIAL</t>
+        </is>
+      </c>
+      <c r="E5" s="34" t="n"/>
+      <c r="F5" s="34" t="n"/>
+      <c r="G5" s="40" t="inlineStr">
+        <is>
+          <t>900785012/911</t>
+        </is>
+      </c>
+      <c r="H5" s="34" t="n"/>
+      <c r="I5" s="46" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J5" s="47" t="n"/>
+      <c r="K5" s="34" t="n"/>
+      <c r="L5" s="34" t="n"/>
+      <c r="M5" s="34" t="n"/>
+      <c r="N5" s="38" t="n"/>
+      <c r="O5" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" s="32">
+      <c r="B6" s="45" t="n"/>
+      <c r="C6" s="34" t="n"/>
+      <c r="D6" s="45" t="n"/>
+      <c r="E6" s="34" t="n"/>
+      <c r="F6" s="34" t="n"/>
+      <c r="G6" s="41" t="inlineStr">
+        <is>
+          <t>DEPOSITO 2 Y 4</t>
+        </is>
+      </c>
+      <c r="H6" s="34" t="n"/>
+      <c r="I6" s="48" t="n"/>
+      <c r="J6" s="47" t="n"/>
+      <c r="K6" s="34" t="n"/>
+      <c r="L6" s="34" t="n"/>
+      <c r="M6" s="34" t="n"/>
+      <c r="N6" s="38" t="n"/>
+      <c r="O6" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="32">
+      <c r="B7" s="45" t="n"/>
+      <c r="C7" s="34" t="n"/>
+      <c r="D7" s="49" t="inlineStr">
+        <is>
+          <t>CARIBERMAR DEL CARIBE</t>
+        </is>
+      </c>
+      <c r="E7" s="34" t="n"/>
+      <c r="F7" s="34" t="n"/>
+      <c r="G7" s="49" t="inlineStr">
+        <is>
+          <t>901380949/911</t>
+        </is>
+      </c>
+      <c r="H7" s="34" t="n"/>
+      <c r="I7" s="48" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J7" s="43" t="n"/>
+      <c r="K7" s="34" t="n"/>
+      <c r="L7" s="34" t="n"/>
+      <c r="M7" s="34" t="n"/>
+      <c r="N7" s="38" t="n"/>
+      <c r="O7" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="8" s="32">
+      <c r="B8" s="50" t="n"/>
+      <c r="C8" s="50" t="n"/>
+      <c r="D8" s="51" t="n"/>
+      <c r="E8" s="50" t="n"/>
+      <c r="F8" s="50" t="n"/>
+      <c r="G8" s="50" t="n"/>
+      <c r="H8" s="51" t="n"/>
+      <c r="I8" s="50" t="n"/>
+      <c r="J8" s="51" t="n"/>
+      <c r="K8" s="51" t="n"/>
+      <c r="L8" s="50" t="n"/>
+      <c r="M8" s="52" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="9" s="32">
+      <c r="B9" s="53" t="inlineStr">
+        <is>
+          <t>ENERGIA ELECTRICA</t>
+        </is>
+      </c>
+      <c r="C9" s="34" t="n"/>
+      <c r="D9" s="34" t="n"/>
+      <c r="E9" s="34" t="n"/>
+      <c r="F9" s="34" t="n"/>
+      <c r="G9" s="34" t="n"/>
+      <c r="H9" s="34" t="n"/>
+      <c r="I9" s="34" t="n"/>
+      <c r="J9" s="34" t="n"/>
+      <c r="K9" s="34" t="n"/>
+      <c r="L9" s="34" t="n"/>
+      <c r="M9" s="34" t="n"/>
+      <c r="N9" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" s="32">
+      <c r="B10" s="54" t="inlineStr">
+        <is>
+          <t>PER.DE COBRO</t>
+        </is>
+      </c>
+      <c r="C10" s="38" t="n"/>
+      <c r="D10" s="54" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="E10" s="34" t="n"/>
+      <c r="F10" s="34" t="n"/>
+      <c r="G10" s="34" t="n"/>
+      <c r="H10" s="38" t="n"/>
+      <c r="I10" s="55" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN PPTOS</t>
+        </is>
+      </c>
+      <c r="J10" s="34" t="n"/>
+      <c r="K10" s="34" t="n"/>
+      <c r="L10" s="34" t="n"/>
+      <c r="M10" s="34" t="n"/>
+      <c r="N10" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="11" s="32">
+      <c r="B11" s="54" t="inlineStr">
+        <is>
+          <t>INICIAL</t>
+        </is>
+      </c>
+      <c r="C11" s="54" t="inlineStr">
+        <is>
+          <t>FINAL</t>
+        </is>
+      </c>
+      <c r="D11" s="54" t="inlineStr">
+        <is>
+          <t>CAUSA</t>
+        </is>
+      </c>
+      <c r="E11" s="54" t="inlineStr">
+        <is>
+          <t>PAGA</t>
+        </is>
+      </c>
+      <c r="F11" s="54" t="inlineStr">
+        <is>
+          <t>AJUS</t>
+        </is>
+      </c>
+      <c r="G11" s="54" t="inlineStr">
+        <is>
+          <t>DOC PAG</t>
+        </is>
+      </c>
+      <c r="H11" s="54" t="inlineStr">
+        <is>
+          <t>DOC AJ</t>
+        </is>
+      </c>
+      <c r="I11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU ACT</t>
+        </is>
+      </c>
+      <c r="J11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU REAC</t>
+        </is>
+      </c>
+      <c r="K11" s="54" t="inlineStr">
+        <is>
+          <t>KW</t>
+        </is>
+      </c>
+      <c r="L11" s="54" t="inlineStr">
+        <is>
+          <t>Vr  KW</t>
+        </is>
+      </c>
+      <c r="M11" s="54" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="N11" s="54" t="inlineStr">
+        <is>
+          <t>ALUMBRADO</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="12" s="32">
+      <c r="B12" s="56" t="n"/>
+      <c r="C12" s="57" t="n"/>
+      <c r="D12" s="57" t="n"/>
+      <c r="E12" s="57" t="n"/>
+      <c r="F12" s="57" t="n"/>
+      <c r="G12" s="57" t="n"/>
+      <c r="H12" s="57" t="n"/>
+      <c r="I12" s="57" t="n"/>
+      <c r="J12" s="57" t="n"/>
+      <c r="K12" s="57" t="n"/>
+      <c r="L12" s="57" t="n"/>
+      <c r="M12" s="57" t="n"/>
+      <c r="N12" s="58" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="13" s="32">
+      <c r="B13" s="59" t="n"/>
+      <c r="N13" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="14" s="32">
+      <c r="B14" s="59" t="n"/>
+      <c r="N14" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" s="32">
+      <c r="B15" s="59" t="n"/>
+      <c r="N15" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="16" s="32">
+      <c r="B16" s="59" t="n"/>
+      <c r="N16" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="17" s="32">
+      <c r="B17" s="59" t="n"/>
+      <c r="N17" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="18" s="32">
+      <c r="B18" s="59" t="n"/>
+      <c r="N18" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" s="32">
+      <c r="B19" s="59" t="n"/>
+      <c r="N19" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="20" s="32">
+      <c r="B20" s="59" t="n"/>
+      <c r="N20" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="21" s="32">
+      <c r="B21" s="59" t="n"/>
+      <c r="N21" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="22" s="32">
+      <c r="B22" s="59" t="n"/>
+      <c r="N22" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="23" s="32">
+      <c r="B23" s="59" t="n"/>
+      <c r="N23" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="24" s="32">
+      <c r="B24" s="61" t="n"/>
+      <c r="C24" s="62" t="n"/>
+      <c r="D24" s="62" t="n"/>
+      <c r="E24" s="62" t="n"/>
+      <c r="F24" s="62" t="n"/>
+      <c r="G24" s="62" t="n"/>
+      <c r="H24" s="62" t="n"/>
+      <c r="I24" s="62" t="n"/>
+      <c r="J24" s="62" t="n"/>
+      <c r="K24" s="62" t="n"/>
+      <c r="L24" s="62" t="n"/>
+      <c r="M24" s="62" t="n"/>
+      <c r="N24" s="63" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="25" s="32"/>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="B9:N9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="I10:N10"/>
+  </mergeCells>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="B2:O24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.18359375" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="31" width="2.57"/>
+    <col customWidth="1" max="2" min="2" style="31" width="12.14"/>
+    <col customWidth="1" max="3" min="3" style="31" width="12.71"/>
+    <col customWidth="1" max="4" min="4" style="31" width="14.15"/>
+    <col customWidth="1" max="5" min="5" style="31" width="13.57"/>
+    <col customWidth="1" max="6" min="6" style="31" width="13.43"/>
+    <col customWidth="1" max="7" min="7" style="31" width="13.29"/>
+    <col customWidth="1" max="8" min="8" style="31" width="13.02"/>
+    <col customWidth="1" max="10" min="9" style="31" width="15.29"/>
+    <col customWidth="1" max="11" min="11" style="31" width="14.28"/>
+    <col customWidth="1" max="12" min="12" style="31" width="15.29"/>
+    <col customWidth="1" max="13" min="13" style="31" width="13.7"/>
+    <col customWidth="1" max="14" min="14" style="31" width="14.15"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15.75" r="1" s="32"/>
+    <row customHeight="1" ht="19.5" r="2" s="32">
+      <c r="B2" s="33" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="C2" s="34" t="n"/>
+      <c r="D2" s="35" t="inlineStr">
+        <is>
+          <t>EMPRESA</t>
+        </is>
+      </c>
+      <c r="E2" s="34" t="n"/>
+      <c r="F2" s="34" t="n"/>
+      <c r="G2" s="35" t="inlineStr">
+        <is>
+          <t>NIT</t>
+        </is>
+      </c>
+      <c r="H2" s="34" t="n"/>
+      <c r="I2" s="36" t="inlineStr">
+        <is>
+          <t>MEDIDOR</t>
+        </is>
+      </c>
+      <c r="J2" s="37" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="K2" s="34" t="n"/>
+      <c r="L2" s="34" t="n"/>
+      <c r="M2" s="34" t="n"/>
+      <c r="N2" s="38" t="n"/>
+      <c r="O2" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="3" s="32">
+      <c r="B3" s="40" t="inlineStr">
+        <is>
+          <t>ENERGIA</t>
+        </is>
+      </c>
+      <c r="C3" s="34" t="n"/>
+      <c r="D3" s="41" t="inlineStr">
+        <is>
+          <t>ELECTRICARIBE</t>
+        </is>
+      </c>
+      <c r="E3" s="34" t="n"/>
+      <c r="F3" s="34" t="n"/>
+      <c r="G3" s="41" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H3" s="34" t="n"/>
+      <c r="I3" s="42" t="n">
+        <v>25782236</v>
+      </c>
+      <c r="J3" s="43" t="inlineStr">
+        <is>
+          <t>CC. PLAZA BOCAGRANDE LOCAL 3-11</t>
+        </is>
+      </c>
+      <c r="K3" s="34" t="n"/>
+      <c r="L3" s="34" t="n"/>
+      <c r="M3" s="34" t="n"/>
+      <c r="N3" s="38" t="n"/>
+      <c r="O3" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" s="32">
+      <c r="B4" s="40" t="n"/>
+      <c r="C4" s="34" t="n"/>
+      <c r="D4" s="40" t="n"/>
+      <c r="E4" s="34" t="n"/>
+      <c r="F4" s="34" t="n"/>
+      <c r="G4" s="40" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H4" s="34" t="n"/>
+      <c r="I4" s="44" t="n">
+        <v>25942309</v>
+      </c>
+      <c r="J4" s="43" t="inlineStr">
+        <is>
+          <t>CR 1 12-120 ENTR BG1 LOC 311</t>
+        </is>
+      </c>
+      <c r="K4" s="34" t="n"/>
+      <c r="L4" s="34" t="n"/>
+      <c r="M4" s="34" t="n"/>
+      <c r="N4" s="38" t="n"/>
+      <c r="O4" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" s="32">
+      <c r="B5" s="45" t="n"/>
+      <c r="C5" s="34" t="n"/>
+      <c r="D5" s="40" t="inlineStr">
+        <is>
+          <t>PLAZA BOCAGRANDE CENTRO COMERCIAL</t>
+        </is>
+      </c>
+      <c r="E5" s="34" t="n"/>
+      <c r="F5" s="34" t="n"/>
+      <c r="G5" s="40" t="inlineStr">
+        <is>
+          <t>900785012/911</t>
+        </is>
+      </c>
+      <c r="H5" s="34" t="n"/>
+      <c r="I5" s="46" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J5" s="47" t="n"/>
+      <c r="K5" s="34" t="n"/>
+      <c r="L5" s="34" t="n"/>
+      <c r="M5" s="34" t="n"/>
+      <c r="N5" s="38" t="n"/>
+      <c r="O5" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" s="32">
+      <c r="B6" s="45" t="n"/>
+      <c r="C6" s="34" t="n"/>
+      <c r="D6" s="45" t="n"/>
+      <c r="E6" s="34" t="n"/>
+      <c r="F6" s="34" t="n"/>
+      <c r="G6" s="41" t="inlineStr">
+        <is>
+          <t>DEPOSITO 2 Y 4</t>
+        </is>
+      </c>
+      <c r="H6" s="34" t="n"/>
+      <c r="I6" s="48" t="n"/>
+      <c r="J6" s="47" t="n"/>
+      <c r="K6" s="34" t="n"/>
+      <c r="L6" s="34" t="n"/>
+      <c r="M6" s="34" t="n"/>
+      <c r="N6" s="38" t="n"/>
+      <c r="O6" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="32">
+      <c r="B7" s="45" t="n"/>
+      <c r="C7" s="34" t="n"/>
+      <c r="D7" s="49" t="inlineStr">
+        <is>
+          <t>CARIBERMAR DEL CARIBE</t>
+        </is>
+      </c>
+      <c r="E7" s="34" t="n"/>
+      <c r="F7" s="34" t="n"/>
+      <c r="G7" s="49" t="inlineStr">
+        <is>
+          <t>901380949/911</t>
+        </is>
+      </c>
+      <c r="H7" s="34" t="n"/>
+      <c r="I7" s="48" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J7" s="43" t="n"/>
+      <c r="K7" s="34" t="n"/>
+      <c r="L7" s="34" t="n"/>
+      <c r="M7" s="34" t="n"/>
+      <c r="N7" s="38" t="n"/>
+      <c r="O7" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="8" s="32">
+      <c r="B8" s="50" t="n"/>
+      <c r="C8" s="50" t="n"/>
+      <c r="D8" s="51" t="n"/>
+      <c r="E8" s="50" t="n"/>
+      <c r="F8" s="50" t="n"/>
+      <c r="G8" s="50" t="n"/>
+      <c r="H8" s="51" t="n"/>
+      <c r="I8" s="50" t="n"/>
+      <c r="J8" s="51" t="n"/>
+      <c r="K8" s="51" t="n"/>
+      <c r="L8" s="50" t="n"/>
+      <c r="M8" s="52" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="9" s="32">
+      <c r="B9" s="53" t="inlineStr">
+        <is>
+          <t>ENERGIA ELECTRICA</t>
+        </is>
+      </c>
+      <c r="C9" s="34" t="n"/>
+      <c r="D9" s="34" t="n"/>
+      <c r="E9" s="34" t="n"/>
+      <c r="F9" s="34" t="n"/>
+      <c r="G9" s="34" t="n"/>
+      <c r="H9" s="34" t="n"/>
+      <c r="I9" s="34" t="n"/>
+      <c r="J9" s="34" t="n"/>
+      <c r="K9" s="34" t="n"/>
+      <c r="L9" s="34" t="n"/>
+      <c r="M9" s="34" t="n"/>
+      <c r="N9" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" s="32">
+      <c r="B10" s="54" t="inlineStr">
+        <is>
+          <t>PER.DE COBRO</t>
+        </is>
+      </c>
+      <c r="C10" s="38" t="n"/>
+      <c r="D10" s="54" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="E10" s="34" t="n"/>
+      <c r="F10" s="34" t="n"/>
+      <c r="G10" s="34" t="n"/>
+      <c r="H10" s="38" t="n"/>
+      <c r="I10" s="55" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN PPTOS</t>
+        </is>
+      </c>
+      <c r="J10" s="34" t="n"/>
+      <c r="K10" s="34" t="n"/>
+      <c r="L10" s="34" t="n"/>
+      <c r="M10" s="34" t="n"/>
+      <c r="N10" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="11" s="32">
+      <c r="B11" s="54" t="inlineStr">
+        <is>
+          <t>INICIAL</t>
+        </is>
+      </c>
+      <c r="C11" s="54" t="inlineStr">
+        <is>
+          <t>FINAL</t>
+        </is>
+      </c>
+      <c r="D11" s="54" t="inlineStr">
+        <is>
+          <t>CAUSA</t>
+        </is>
+      </c>
+      <c r="E11" s="54" t="inlineStr">
+        <is>
+          <t>PAGA</t>
+        </is>
+      </c>
+      <c r="F11" s="54" t="inlineStr">
+        <is>
+          <t>AJUS</t>
+        </is>
+      </c>
+      <c r="G11" s="54" t="inlineStr">
+        <is>
+          <t>DOC PAG</t>
+        </is>
+      </c>
+      <c r="H11" s="54" t="inlineStr">
+        <is>
+          <t>DOC AJ</t>
+        </is>
+      </c>
+      <c r="I11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU ACT</t>
+        </is>
+      </c>
+      <c r="J11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU REAC</t>
+        </is>
+      </c>
+      <c r="K11" s="54" t="inlineStr">
+        <is>
+          <t>KW</t>
+        </is>
+      </c>
+      <c r="L11" s="54" t="inlineStr">
+        <is>
+          <t>Vr  KW</t>
+        </is>
+      </c>
+      <c r="M11" s="54" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="N11" s="54" t="inlineStr">
+        <is>
+          <t>ALUMBRADO</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="12" s="32">
+      <c r="B12" s="56" t="n"/>
+      <c r="C12" s="57" t="n"/>
+      <c r="D12" s="57" t="n"/>
+      <c r="E12" s="57" t="n"/>
+      <c r="F12" s="57" t="n"/>
+      <c r="G12" s="57" t="n"/>
+      <c r="H12" s="57" t="n"/>
+      <c r="I12" s="57" t="n"/>
+      <c r="J12" s="57" t="n"/>
+      <c r="K12" s="57" t="n"/>
+      <c r="L12" s="57" t="n"/>
+      <c r="M12" s="57" t="n"/>
+      <c r="N12" s="58" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="13" s="32">
+      <c r="B13" s="59" t="n"/>
+      <c r="N13" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="14" s="32">
+      <c r="B14" s="59" t="n"/>
+      <c r="N14" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" s="32">
+      <c r="B15" s="59" t="n"/>
+      <c r="N15" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="16" s="32">
+      <c r="B16" s="59" t="n"/>
+      <c r="N16" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="17" s="32">
+      <c r="B17" s="59" t="n"/>
+      <c r="N17" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="18" s="32">
+      <c r="B18" s="59" t="n"/>
+      <c r="N18" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" s="32">
+      <c r="B19" s="59" t="n"/>
+      <c r="N19" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="20" s="32">
+      <c r="B20" s="59" t="n"/>
+      <c r="N20" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="21" s="32">
+      <c r="B21" s="59" t="n"/>
+      <c r="N21" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="22" s="32">
+      <c r="B22" s="59" t="n"/>
+      <c r="N22" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="23" s="32">
+      <c r="B23" s="59" t="n"/>
+      <c r="N23" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="24" s="32">
+      <c r="B24" s="61" t="n"/>
+      <c r="C24" s="62" t="n"/>
+      <c r="D24" s="62" t="n"/>
+      <c r="E24" s="62" t="n"/>
+      <c r="F24" s="62" t="n"/>
+      <c r="G24" s="62" t="n"/>
+      <c r="H24" s="62" t="n"/>
+      <c r="I24" s="62" t="n"/>
+      <c r="J24" s="62" t="n"/>
+      <c r="K24" s="62" t="n"/>
+      <c r="L24" s="62" t="n"/>
+      <c r="M24" s="62" t="n"/>
+      <c r="N24" s="63" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="25" s="32"/>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="B9:N9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="I10:N10"/>
+  </mergeCells>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="B2:O24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.18359375" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="31" width="2.57"/>
+    <col customWidth="1" max="2" min="2" style="31" width="12.14"/>
+    <col customWidth="1" max="3" min="3" style="31" width="12.71"/>
+    <col customWidth="1" max="4" min="4" style="31" width="14.15"/>
+    <col customWidth="1" max="5" min="5" style="31" width="13.57"/>
+    <col customWidth="1" max="6" min="6" style="31" width="13.43"/>
+    <col customWidth="1" max="7" min="7" style="31" width="13.29"/>
+    <col customWidth="1" max="8" min="8" style="31" width="13.02"/>
+    <col customWidth="1" max="10" min="9" style="31" width="15.29"/>
+    <col customWidth="1" max="11" min="11" style="31" width="14.28"/>
+    <col customWidth="1" max="12" min="12" style="31" width="15.29"/>
+    <col customWidth="1" max="13" min="13" style="31" width="13.7"/>
+    <col customWidth="1" max="14" min="14" style="31" width="14.15"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15.75" r="1" s="32"/>
+    <row customHeight="1" ht="19.5" r="2" s="32">
+      <c r="B2" s="33" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="C2" s="34" t="n"/>
+      <c r="D2" s="35" t="inlineStr">
+        <is>
+          <t>EMPRESA</t>
+        </is>
+      </c>
+      <c r="E2" s="34" t="n"/>
+      <c r="F2" s="34" t="n"/>
+      <c r="G2" s="35" t="inlineStr">
+        <is>
+          <t>NIT</t>
+        </is>
+      </c>
+      <c r="H2" s="34" t="n"/>
+      <c r="I2" s="36" t="inlineStr">
+        <is>
+          <t>MEDIDOR</t>
+        </is>
+      </c>
+      <c r="J2" s="37" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="K2" s="34" t="n"/>
+      <c r="L2" s="34" t="n"/>
+      <c r="M2" s="34" t="n"/>
+      <c r="N2" s="38" t="n"/>
+      <c r="O2" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="3" s="32">
+      <c r="B3" s="40" t="inlineStr">
+        <is>
+          <t>ENERGIA</t>
+        </is>
+      </c>
+      <c r="C3" s="34" t="n"/>
+      <c r="D3" s="41" t="inlineStr">
+        <is>
+          <t>ELECTRICARIBE</t>
+        </is>
+      </c>
+      <c r="E3" s="34" t="n"/>
+      <c r="F3" s="34" t="n"/>
+      <c r="G3" s="41" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H3" s="34" t="n"/>
+      <c r="I3" s="42" t="n">
+        <v>25782236</v>
+      </c>
+      <c r="J3" s="43" t="inlineStr">
+        <is>
+          <t>CC. PLAZA BOCAGRANDE LOCAL 3-11</t>
+        </is>
+      </c>
+      <c r="K3" s="34" t="n"/>
+      <c r="L3" s="34" t="n"/>
+      <c r="M3" s="34" t="n"/>
+      <c r="N3" s="38" t="n"/>
+      <c r="O3" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" s="32">
+      <c r="B4" s="40" t="n"/>
+      <c r="C4" s="34" t="n"/>
+      <c r="D4" s="40" t="n"/>
+      <c r="E4" s="34" t="n"/>
+      <c r="F4" s="34" t="n"/>
+      <c r="G4" s="40" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H4" s="34" t="n"/>
+      <c r="I4" s="44" t="n">
+        <v>25942309</v>
+      </c>
+      <c r="J4" s="43" t="inlineStr">
+        <is>
+          <t>CR 1 12-120 ENTR BG1 LOC 311</t>
+        </is>
+      </c>
+      <c r="K4" s="34" t="n"/>
+      <c r="L4" s="34" t="n"/>
+      <c r="M4" s="34" t="n"/>
+      <c r="N4" s="38" t="n"/>
+      <c r="O4" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" s="32">
+      <c r="B5" s="45" t="n"/>
+      <c r="C5" s="34" t="n"/>
+      <c r="D5" s="40" t="inlineStr">
+        <is>
+          <t>PLAZA BOCAGRANDE CENTRO COMERCIAL</t>
+        </is>
+      </c>
+      <c r="E5" s="34" t="n"/>
+      <c r="F5" s="34" t="n"/>
+      <c r="G5" s="40" t="inlineStr">
+        <is>
+          <t>900785012/911</t>
+        </is>
+      </c>
+      <c r="H5" s="34" t="n"/>
+      <c r="I5" s="46" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J5" s="47" t="n"/>
+      <c r="K5" s="34" t="n"/>
+      <c r="L5" s="34" t="n"/>
+      <c r="M5" s="34" t="n"/>
+      <c r="N5" s="38" t="n"/>
+      <c r="O5" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" s="32">
+      <c r="B6" s="45" t="n"/>
+      <c r="C6" s="34" t="n"/>
+      <c r="D6" s="45" t="n"/>
+      <c r="E6" s="34" t="n"/>
+      <c r="F6" s="34" t="n"/>
+      <c r="G6" s="41" t="inlineStr">
+        <is>
+          <t>DEPOSITO 2 Y 4</t>
+        </is>
+      </c>
+      <c r="H6" s="34" t="n"/>
+      <c r="I6" s="48" t="n"/>
+      <c r="J6" s="47" t="n"/>
+      <c r="K6" s="34" t="n"/>
+      <c r="L6" s="34" t="n"/>
+      <c r="M6" s="34" t="n"/>
+      <c r="N6" s="38" t="n"/>
+      <c r="O6" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="32">
+      <c r="B7" s="45" t="n"/>
+      <c r="C7" s="34" t="n"/>
+      <c r="D7" s="49" t="inlineStr">
+        <is>
+          <t>CARIBERMAR DEL CARIBE</t>
+        </is>
+      </c>
+      <c r="E7" s="34" t="n"/>
+      <c r="F7" s="34" t="n"/>
+      <c r="G7" s="49" t="inlineStr">
+        <is>
+          <t>901380949/911</t>
+        </is>
+      </c>
+      <c r="H7" s="34" t="n"/>
+      <c r="I7" s="48" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J7" s="43" t="n"/>
+      <c r="K7" s="34" t="n"/>
+      <c r="L7" s="34" t="n"/>
+      <c r="M7" s="34" t="n"/>
+      <c r="N7" s="38" t="n"/>
+      <c r="O7" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="8" s="32">
+      <c r="B8" s="50" t="n"/>
+      <c r="C8" s="50" t="n"/>
+      <c r="D8" s="51" t="n"/>
+      <c r="E8" s="50" t="n"/>
+      <c r="F8" s="50" t="n"/>
+      <c r="G8" s="50" t="n"/>
+      <c r="H8" s="51" t="n"/>
+      <c r="I8" s="50" t="n"/>
+      <c r="J8" s="51" t="n"/>
+      <c r="K8" s="51" t="n"/>
+      <c r="L8" s="50" t="n"/>
+      <c r="M8" s="52" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="9" s="32">
+      <c r="B9" s="53" t="inlineStr">
+        <is>
+          <t>ENERGIA ELECTRICA</t>
+        </is>
+      </c>
+      <c r="C9" s="34" t="n"/>
+      <c r="D9" s="34" t="n"/>
+      <c r="E9" s="34" t="n"/>
+      <c r="F9" s="34" t="n"/>
+      <c r="G9" s="34" t="n"/>
+      <c r="H9" s="34" t="n"/>
+      <c r="I9" s="34" t="n"/>
+      <c r="J9" s="34" t="n"/>
+      <c r="K9" s="34" t="n"/>
+      <c r="L9" s="34" t="n"/>
+      <c r="M9" s="34" t="n"/>
+      <c r="N9" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" s="32">
+      <c r="B10" s="54" t="inlineStr">
+        <is>
+          <t>PER.DE COBRO</t>
+        </is>
+      </c>
+      <c r="C10" s="38" t="n"/>
+      <c r="D10" s="54" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="E10" s="34" t="n"/>
+      <c r="F10" s="34" t="n"/>
+      <c r="G10" s="34" t="n"/>
+      <c r="H10" s="38" t="n"/>
+      <c r="I10" s="55" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN PPTOS</t>
+        </is>
+      </c>
+      <c r="J10" s="34" t="n"/>
+      <c r="K10" s="34" t="n"/>
+      <c r="L10" s="34" t="n"/>
+      <c r="M10" s="34" t="n"/>
+      <c r="N10" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="11" s="32">
+      <c r="B11" s="54" t="inlineStr">
+        <is>
+          <t>INICIAL</t>
+        </is>
+      </c>
+      <c r="C11" s="54" t="inlineStr">
+        <is>
+          <t>FINAL</t>
+        </is>
+      </c>
+      <c r="D11" s="54" t="inlineStr">
+        <is>
+          <t>CAUSA</t>
+        </is>
+      </c>
+      <c r="E11" s="54" t="inlineStr">
+        <is>
+          <t>PAGA</t>
+        </is>
+      </c>
+      <c r="F11" s="54" t="inlineStr">
+        <is>
+          <t>AJUS</t>
+        </is>
+      </c>
+      <c r="G11" s="54" t="inlineStr">
+        <is>
+          <t>DOC PAG</t>
+        </is>
+      </c>
+      <c r="H11" s="54" t="inlineStr">
+        <is>
+          <t>DOC AJ</t>
+        </is>
+      </c>
+      <c r="I11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU ACT</t>
+        </is>
+      </c>
+      <c r="J11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU REAC</t>
+        </is>
+      </c>
+      <c r="K11" s="54" t="inlineStr">
+        <is>
+          <t>KW</t>
+        </is>
+      </c>
+      <c r="L11" s="54" t="inlineStr">
+        <is>
+          <t>Vr  KW</t>
+        </is>
+      </c>
+      <c r="M11" s="54" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="N11" s="54" t="inlineStr">
+        <is>
+          <t>ALUMBRADO</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="12" s="32">
+      <c r="B12" s="56" t="n"/>
+      <c r="C12" s="57" t="n"/>
+      <c r="D12" s="57" t="n"/>
+      <c r="E12" s="57" t="n"/>
+      <c r="F12" s="57" t="n"/>
+      <c r="G12" s="57" t="n"/>
+      <c r="H12" s="57" t="n"/>
+      <c r="I12" s="57" t="n"/>
+      <c r="J12" s="57" t="n"/>
+      <c r="K12" s="57" t="n"/>
+      <c r="L12" s="57" t="n"/>
+      <c r="M12" s="57" t="n"/>
+      <c r="N12" s="58" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="13" s="32">
+      <c r="B13" s="59" t="n"/>
+      <c r="N13" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="14" s="32">
+      <c r="B14" s="59" t="n"/>
+      <c r="N14" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" s="32">
+      <c r="B15" s="59" t="n"/>
+      <c r="N15" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="16" s="32">
+      <c r="B16" s="59" t="n"/>
+      <c r="N16" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="17" s="32">
+      <c r="B17" s="59" t="n"/>
+      <c r="N17" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="18" s="32">
+      <c r="B18" s="59" t="n"/>
+      <c r="N18" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" s="32">
+      <c r="B19" s="59" t="n"/>
+      <c r="N19" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="20" s="32">
+      <c r="B20" s="59" t="n"/>
+      <c r="N20" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="21" s="32">
+      <c r="B21" s="59" t="n"/>
+      <c r="N21" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="22" s="32">
+      <c r="B22" s="59" t="n"/>
+      <c r="N22" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="23" s="32">
+      <c r="B23" s="59" t="n"/>
+      <c r="N23" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="24" s="32">
+      <c r="B24" s="61" t="n"/>
+      <c r="C24" s="62" t="n"/>
+      <c r="D24" s="62" t="n"/>
+      <c r="E24" s="62" t="n"/>
+      <c r="F24" s="62" t="n"/>
+      <c r="G24" s="62" t="n"/>
+      <c r="H24" s="62" t="n"/>
+      <c r="I24" s="62" t="n"/>
+      <c r="J24" s="62" t="n"/>
+      <c r="K24" s="62" t="n"/>
+      <c r="L24" s="62" t="n"/>
+      <c r="M24" s="62" t="n"/>
+      <c r="N24" s="63" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="25" s="32"/>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="B9:N9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="I10:N10"/>
+  </mergeCells>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="B2:O24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.18359375" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="31" width="2.57"/>
+    <col customWidth="1" max="2" min="2" style="31" width="12.14"/>
+    <col customWidth="1" max="3" min="3" style="31" width="12.71"/>
+    <col customWidth="1" max="4" min="4" style="31" width="14.15"/>
+    <col customWidth="1" max="5" min="5" style="31" width="13.57"/>
+    <col customWidth="1" max="6" min="6" style="31" width="13.43"/>
+    <col customWidth="1" max="7" min="7" style="31" width="13.29"/>
+    <col customWidth="1" max="8" min="8" style="31" width="13.02"/>
+    <col customWidth="1" max="10" min="9" style="31" width="15.29"/>
+    <col customWidth="1" max="11" min="11" style="31" width="14.28"/>
+    <col customWidth="1" max="12" min="12" style="31" width="15.29"/>
+    <col customWidth="1" max="13" min="13" style="31" width="13.7"/>
+    <col customWidth="1" max="14" min="14" style="31" width="14.15"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15.75" r="1" s="32"/>
+    <row customHeight="1" ht="19.5" r="2" s="32">
+      <c r="B2" s="33" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="C2" s="34" t="n"/>
+      <c r="D2" s="35" t="inlineStr">
+        <is>
+          <t>EMPRESA</t>
+        </is>
+      </c>
+      <c r="E2" s="34" t="n"/>
+      <c r="F2" s="34" t="n"/>
+      <c r="G2" s="35" t="inlineStr">
+        <is>
+          <t>NIT</t>
+        </is>
+      </c>
+      <c r="H2" s="34" t="n"/>
+      <c r="I2" s="36" t="inlineStr">
+        <is>
+          <t>MEDIDOR</t>
+        </is>
+      </c>
+      <c r="J2" s="37" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="K2" s="34" t="n"/>
+      <c r="L2" s="34" t="n"/>
+      <c r="M2" s="34" t="n"/>
+      <c r="N2" s="38" t="n"/>
+      <c r="O2" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="3" s="32">
+      <c r="B3" s="40" t="inlineStr">
+        <is>
+          <t>ENERGIA</t>
+        </is>
+      </c>
+      <c r="C3" s="34" t="n"/>
+      <c r="D3" s="41" t="inlineStr">
+        <is>
+          <t>ELECTRICARIBE</t>
+        </is>
+      </c>
+      <c r="E3" s="34" t="n"/>
+      <c r="F3" s="34" t="n"/>
+      <c r="G3" s="41" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H3" s="34" t="n"/>
+      <c r="I3" s="42" t="n">
+        <v>25782236</v>
+      </c>
+      <c r="J3" s="43" t="inlineStr">
+        <is>
+          <t>CC. PLAZA BOCAGRANDE LOCAL 3-11</t>
+        </is>
+      </c>
+      <c r="K3" s="34" t="n"/>
+      <c r="L3" s="34" t="n"/>
+      <c r="M3" s="34" t="n"/>
+      <c r="N3" s="38" t="n"/>
+      <c r="O3" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" s="32">
+      <c r="B4" s="40" t="n"/>
+      <c r="C4" s="34" t="n"/>
+      <c r="D4" s="40" t="n"/>
+      <c r="E4" s="34" t="n"/>
+      <c r="F4" s="34" t="n"/>
+      <c r="G4" s="40" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H4" s="34" t="n"/>
+      <c r="I4" s="44" t="n">
+        <v>25942309</v>
+      </c>
+      <c r="J4" s="43" t="inlineStr">
+        <is>
+          <t>CR 1 12-120 ENTR BG1 LOC 311</t>
+        </is>
+      </c>
+      <c r="K4" s="34" t="n"/>
+      <c r="L4" s="34" t="n"/>
+      <c r="M4" s="34" t="n"/>
+      <c r="N4" s="38" t="n"/>
+      <c r="O4" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" s="32">
+      <c r="B5" s="45" t="n"/>
+      <c r="C5" s="34" t="n"/>
+      <c r="D5" s="40" t="inlineStr">
+        <is>
+          <t>PLAZA BOCAGRANDE CENTRO COMERCIAL</t>
+        </is>
+      </c>
+      <c r="E5" s="34" t="n"/>
+      <c r="F5" s="34" t="n"/>
+      <c r="G5" s="40" t="inlineStr">
+        <is>
+          <t>900785012/911</t>
+        </is>
+      </c>
+      <c r="H5" s="34" t="n"/>
+      <c r="I5" s="46" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J5" s="47" t="n"/>
+      <c r="K5" s="34" t="n"/>
+      <c r="L5" s="34" t="n"/>
+      <c r="M5" s="34" t="n"/>
+      <c r="N5" s="38" t="n"/>
+      <c r="O5" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" s="32">
+      <c r="B6" s="45" t="n"/>
+      <c r="C6" s="34" t="n"/>
+      <c r="D6" s="45" t="n"/>
+      <c r="E6" s="34" t="n"/>
+      <c r="F6" s="34" t="n"/>
+      <c r="G6" s="41" t="inlineStr">
+        <is>
+          <t>DEPOSITO 2 Y 4</t>
+        </is>
+      </c>
+      <c r="H6" s="34" t="n"/>
+      <c r="I6" s="48" t="n"/>
+      <c r="J6" s="47" t="n"/>
+      <c r="K6" s="34" t="n"/>
+      <c r="L6" s="34" t="n"/>
+      <c r="M6" s="34" t="n"/>
+      <c r="N6" s="38" t="n"/>
+      <c r="O6" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="32">
+      <c r="B7" s="45" t="n"/>
+      <c r="C7" s="34" t="n"/>
+      <c r="D7" s="49" t="inlineStr">
+        <is>
+          <t>CARIBERMAR DEL CARIBE</t>
+        </is>
+      </c>
+      <c r="E7" s="34" t="n"/>
+      <c r="F7" s="34" t="n"/>
+      <c r="G7" s="49" t="inlineStr">
+        <is>
+          <t>901380949/911</t>
+        </is>
+      </c>
+      <c r="H7" s="34" t="n"/>
+      <c r="I7" s="48" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J7" s="43" t="n"/>
+      <c r="K7" s="34" t="n"/>
+      <c r="L7" s="34" t="n"/>
+      <c r="M7" s="34" t="n"/>
+      <c r="N7" s="38" t="n"/>
+      <c r="O7" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="8" s="32">
+      <c r="B8" s="50" t="n"/>
+      <c r="C8" s="50" t="n"/>
+      <c r="D8" s="51" t="n"/>
+      <c r="E8" s="50" t="n"/>
+      <c r="F8" s="50" t="n"/>
+      <c r="G8" s="50" t="n"/>
+      <c r="H8" s="51" t="n"/>
+      <c r="I8" s="50" t="n"/>
+      <c r="J8" s="51" t="n"/>
+      <c r="K8" s="51" t="n"/>
+      <c r="L8" s="50" t="n"/>
+      <c r="M8" s="52" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="9" s="32">
+      <c r="B9" s="53" t="inlineStr">
+        <is>
+          <t>ENERGIA ELECTRICA</t>
+        </is>
+      </c>
+      <c r="C9" s="34" t="n"/>
+      <c r="D9" s="34" t="n"/>
+      <c r="E9" s="34" t="n"/>
+      <c r="F9" s="34" t="n"/>
+      <c r="G9" s="34" t="n"/>
+      <c r="H9" s="34" t="n"/>
+      <c r="I9" s="34" t="n"/>
+      <c r="J9" s="34" t="n"/>
+      <c r="K9" s="34" t="n"/>
+      <c r="L9" s="34" t="n"/>
+      <c r="M9" s="34" t="n"/>
+      <c r="N9" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" s="32">
+      <c r="B10" s="54" t="inlineStr">
+        <is>
+          <t>PER.DE COBRO</t>
+        </is>
+      </c>
+      <c r="C10" s="38" t="n"/>
+      <c r="D10" s="54" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="E10" s="34" t="n"/>
+      <c r="F10" s="34" t="n"/>
+      <c r="G10" s="34" t="n"/>
+      <c r="H10" s="38" t="n"/>
+      <c r="I10" s="55" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN PPTOS</t>
+        </is>
+      </c>
+      <c r="J10" s="34" t="n"/>
+      <c r="K10" s="34" t="n"/>
+      <c r="L10" s="34" t="n"/>
+      <c r="M10" s="34" t="n"/>
+      <c r="N10" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="11" s="32">
+      <c r="B11" s="54" t="inlineStr">
+        <is>
+          <t>INICIAL</t>
+        </is>
+      </c>
+      <c r="C11" s="54" t="inlineStr">
+        <is>
+          <t>FINAL</t>
+        </is>
+      </c>
+      <c r="D11" s="54" t="inlineStr">
+        <is>
+          <t>CAUSA</t>
+        </is>
+      </c>
+      <c r="E11" s="54" t="inlineStr">
+        <is>
+          <t>PAGA</t>
+        </is>
+      </c>
+      <c r="F11" s="54" t="inlineStr">
+        <is>
+          <t>AJUS</t>
+        </is>
+      </c>
+      <c r="G11" s="54" t="inlineStr">
+        <is>
+          <t>DOC PAG</t>
+        </is>
+      </c>
+      <c r="H11" s="54" t="inlineStr">
+        <is>
+          <t>DOC AJ</t>
+        </is>
+      </c>
+      <c r="I11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU ACT</t>
+        </is>
+      </c>
+      <c r="J11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU REAC</t>
+        </is>
+      </c>
+      <c r="K11" s="54" t="inlineStr">
+        <is>
+          <t>KW</t>
+        </is>
+      </c>
+      <c r="L11" s="54" t="inlineStr">
+        <is>
+          <t>Vr  KW</t>
+        </is>
+      </c>
+      <c r="M11" s="54" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="N11" s="54" t="inlineStr">
+        <is>
+          <t>ALUMBRADO</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="12" s="32">
+      <c r="B12" s="56" t="n"/>
+      <c r="C12" s="57" t="n"/>
+      <c r="D12" s="57" t="n"/>
+      <c r="E12" s="57" t="n"/>
+      <c r="F12" s="57" t="n"/>
+      <c r="G12" s="57" t="n"/>
+      <c r="H12" s="57" t="n"/>
+      <c r="I12" s="57" t="n"/>
+      <c r="J12" s="57" t="n"/>
+      <c r="K12" s="57" t="n"/>
+      <c r="L12" s="57" t="n"/>
+      <c r="M12" s="57" t="n"/>
+      <c r="N12" s="58" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="13" s="32">
+      <c r="B13" s="59" t="n"/>
+      <c r="N13" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="14" s="32">
+      <c r="B14" s="59" t="n"/>
+      <c r="N14" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" s="32">
+      <c r="B15" s="59" t="n"/>
+      <c r="N15" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="16" s="32">
+      <c r="B16" s="59" t="n"/>
+      <c r="N16" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="17" s="32">
+      <c r="B17" s="59" t="n"/>
+      <c r="N17" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="18" s="32">
+      <c r="B18" s="59" t="n"/>
+      <c r="N18" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" s="32">
+      <c r="B19" s="59" t="n"/>
+      <c r="N19" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="20" s="32">
+      <c r="B20" s="59" t="n"/>
+      <c r="N20" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="21" s="32">
+      <c r="B21" s="59" t="n"/>
+      <c r="N21" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="22" s="32">
+      <c r="B22" s="59" t="n"/>
+      <c r="N22" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="23" s="32">
+      <c r="B23" s="59" t="n"/>
+      <c r="N23" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="24" s="32">
+      <c r="B24" s="61" t="n"/>
+      <c r="C24" s="62" t="n"/>
+      <c r="D24" s="62" t="n"/>
+      <c r="E24" s="62" t="n"/>
+      <c r="F24" s="62" t="n"/>
+      <c r="G24" s="62" t="n"/>
+      <c r="H24" s="62" t="n"/>
+      <c r="I24" s="62" t="n"/>
+      <c r="J24" s="62" t="n"/>
+      <c r="K24" s="62" t="n"/>
+      <c r="L24" s="62" t="n"/>
+      <c r="M24" s="62" t="n"/>
+      <c r="N24" s="63" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="25" s="32"/>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="B9:N9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="I10:N10"/>
+  </mergeCells>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="B2:O24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.18359375" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="31" width="2.57"/>
+    <col customWidth="1" max="2" min="2" style="31" width="12.14"/>
+    <col customWidth="1" max="3" min="3" style="31" width="12.71"/>
+    <col customWidth="1" max="4" min="4" style="31" width="14.15"/>
+    <col customWidth="1" max="5" min="5" style="31" width="13.57"/>
+    <col customWidth="1" max="6" min="6" style="31" width="13.43"/>
+    <col customWidth="1" max="7" min="7" style="31" width="13.29"/>
+    <col customWidth="1" max="8" min="8" style="31" width="13.02"/>
+    <col customWidth="1" max="10" min="9" style="31" width="15.29"/>
+    <col customWidth="1" max="11" min="11" style="31" width="14.28"/>
+    <col customWidth="1" max="12" min="12" style="31" width="15.29"/>
+    <col customWidth="1" max="13" min="13" style="31" width="13.7"/>
+    <col customWidth="1" max="14" min="14" style="31" width="14.15"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15.75" r="1" s="32"/>
+    <row customHeight="1" ht="19.5" r="2" s="32">
+      <c r="B2" s="33" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="C2" s="34" t="n"/>
+      <c r="D2" s="35" t="inlineStr">
+        <is>
+          <t>EMPRESA</t>
+        </is>
+      </c>
+      <c r="E2" s="34" t="n"/>
+      <c r="F2" s="34" t="n"/>
+      <c r="G2" s="35" t="inlineStr">
+        <is>
+          <t>NIT</t>
+        </is>
+      </c>
+      <c r="H2" s="34" t="n"/>
+      <c r="I2" s="36" t="inlineStr">
+        <is>
+          <t>MEDIDOR</t>
+        </is>
+      </c>
+      <c r="J2" s="37" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="K2" s="34" t="n"/>
+      <c r="L2" s="34" t="n"/>
+      <c r="M2" s="34" t="n"/>
+      <c r="N2" s="38" t="n"/>
+      <c r="O2" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="3" s="32">
+      <c r="B3" s="40" t="inlineStr">
+        <is>
+          <t>ENERGIA</t>
+        </is>
+      </c>
+      <c r="C3" s="34" t="n"/>
+      <c r="D3" s="41" t="inlineStr">
+        <is>
+          <t>ELECTRICARIBE</t>
+        </is>
+      </c>
+      <c r="E3" s="34" t="n"/>
+      <c r="F3" s="34" t="n"/>
+      <c r="G3" s="41" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H3" s="34" t="n"/>
+      <c r="I3" s="42" t="n">
+        <v>25782236</v>
+      </c>
+      <c r="J3" s="43" t="inlineStr">
+        <is>
+          <t>CC. PLAZA BOCAGRANDE LOCAL 3-11</t>
+        </is>
+      </c>
+      <c r="K3" s="34" t="n"/>
+      <c r="L3" s="34" t="n"/>
+      <c r="M3" s="34" t="n"/>
+      <c r="N3" s="38" t="n"/>
+      <c r="O3" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" s="32">
+      <c r="B4" s="40" t="n"/>
+      <c r="C4" s="34" t="n"/>
+      <c r="D4" s="40" t="n"/>
+      <c r="E4" s="34" t="n"/>
+      <c r="F4" s="34" t="n"/>
+      <c r="G4" s="40" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H4" s="34" t="n"/>
+      <c r="I4" s="44" t="n">
+        <v>25942309</v>
+      </c>
+      <c r="J4" s="43" t="inlineStr">
+        <is>
+          <t>CR 1 12-120 ENTR BG1 LOC 311</t>
+        </is>
+      </c>
+      <c r="K4" s="34" t="n"/>
+      <c r="L4" s="34" t="n"/>
+      <c r="M4" s="34" t="n"/>
+      <c r="N4" s="38" t="n"/>
+      <c r="O4" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" s="32">
+      <c r="B5" s="45" t="n"/>
+      <c r="C5" s="34" t="n"/>
+      <c r="D5" s="40" t="inlineStr">
+        <is>
+          <t>PLAZA BOCAGRANDE CENTRO COMERCIAL</t>
+        </is>
+      </c>
+      <c r="E5" s="34" t="n"/>
+      <c r="F5" s="34" t="n"/>
+      <c r="G5" s="40" t="inlineStr">
+        <is>
+          <t>900785012/911</t>
+        </is>
+      </c>
+      <c r="H5" s="34" t="n"/>
+      <c r="I5" s="46" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J5" s="47" t="n"/>
+      <c r="K5" s="34" t="n"/>
+      <c r="L5" s="34" t="n"/>
+      <c r="M5" s="34" t="n"/>
+      <c r="N5" s="38" t="n"/>
+      <c r="O5" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" s="32">
+      <c r="B6" s="45" t="n"/>
+      <c r="C6" s="34" t="n"/>
+      <c r="D6" s="45" t="n"/>
+      <c r="E6" s="34" t="n"/>
+      <c r="F6" s="34" t="n"/>
+      <c r="G6" s="41" t="inlineStr">
+        <is>
+          <t>DEPOSITO 2 Y 4</t>
+        </is>
+      </c>
+      <c r="H6" s="34" t="n"/>
+      <c r="I6" s="48" t="n"/>
+      <c r="J6" s="47" t="n"/>
+      <c r="K6" s="34" t="n"/>
+      <c r="L6" s="34" t="n"/>
+      <c r="M6" s="34" t="n"/>
+      <c r="N6" s="38" t="n"/>
+      <c r="O6" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="32">
+      <c r="B7" s="45" t="n"/>
+      <c r="C7" s="34" t="n"/>
+      <c r="D7" s="49" t="inlineStr">
+        <is>
+          <t>CARIBERMAR DEL CARIBE</t>
+        </is>
+      </c>
+      <c r="E7" s="34" t="n"/>
+      <c r="F7" s="34" t="n"/>
+      <c r="G7" s="49" t="inlineStr">
+        <is>
+          <t>901380949/911</t>
+        </is>
+      </c>
+      <c r="H7" s="34" t="n"/>
+      <c r="I7" s="48" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J7" s="43" t="n"/>
+      <c r="K7" s="34" t="n"/>
+      <c r="L7" s="34" t="n"/>
+      <c r="M7" s="34" t="n"/>
+      <c r="N7" s="38" t="n"/>
+      <c r="O7" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="8" s="32">
+      <c r="B8" s="50" t="n"/>
+      <c r="C8" s="50" t="n"/>
+      <c r="D8" s="51" t="n"/>
+      <c r="E8" s="50" t="n"/>
+      <c r="F8" s="50" t="n"/>
+      <c r="G8" s="50" t="n"/>
+      <c r="H8" s="51" t="n"/>
+      <c r="I8" s="50" t="n"/>
+      <c r="J8" s="51" t="n"/>
+      <c r="K8" s="51" t="n"/>
+      <c r="L8" s="50" t="n"/>
+      <c r="M8" s="52" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="9" s="32">
+      <c r="B9" s="53" t="inlineStr">
+        <is>
+          <t>ENERGIA ELECTRICA</t>
+        </is>
+      </c>
+      <c r="C9" s="34" t="n"/>
+      <c r="D9" s="34" t="n"/>
+      <c r="E9" s="34" t="n"/>
+      <c r="F9" s="34" t="n"/>
+      <c r="G9" s="34" t="n"/>
+      <c r="H9" s="34" t="n"/>
+      <c r="I9" s="34" t="n"/>
+      <c r="J9" s="34" t="n"/>
+      <c r="K9" s="34" t="n"/>
+      <c r="L9" s="34" t="n"/>
+      <c r="M9" s="34" t="n"/>
+      <c r="N9" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" s="32">
+      <c r="B10" s="54" t="inlineStr">
+        <is>
+          <t>PER.DE COBRO</t>
+        </is>
+      </c>
+      <c r="C10" s="38" t="n"/>
+      <c r="D10" s="54" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="E10" s="34" t="n"/>
+      <c r="F10" s="34" t="n"/>
+      <c r="G10" s="34" t="n"/>
+      <c r="H10" s="38" t="n"/>
+      <c r="I10" s="55" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN PPTOS</t>
+        </is>
+      </c>
+      <c r="J10" s="34" t="n"/>
+      <c r="K10" s="34" t="n"/>
+      <c r="L10" s="34" t="n"/>
+      <c r="M10" s="34" t="n"/>
+      <c r="N10" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="11" s="32">
+      <c r="B11" s="54" t="inlineStr">
+        <is>
+          <t>INICIAL</t>
+        </is>
+      </c>
+      <c r="C11" s="54" t="inlineStr">
+        <is>
+          <t>FINAL</t>
+        </is>
+      </c>
+      <c r="D11" s="54" t="inlineStr">
+        <is>
+          <t>CAUSA</t>
+        </is>
+      </c>
+      <c r="E11" s="54" t="inlineStr">
+        <is>
+          <t>PAGA</t>
+        </is>
+      </c>
+      <c r="F11" s="54" t="inlineStr">
+        <is>
+          <t>AJUS</t>
+        </is>
+      </c>
+      <c r="G11" s="54" t="inlineStr">
+        <is>
+          <t>DOC PAG</t>
+        </is>
+      </c>
+      <c r="H11" s="54" t="inlineStr">
+        <is>
+          <t>DOC AJ</t>
+        </is>
+      </c>
+      <c r="I11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU ACT</t>
+        </is>
+      </c>
+      <c r="J11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU REAC</t>
+        </is>
+      </c>
+      <c r="K11" s="54" t="inlineStr">
+        <is>
+          <t>KW</t>
+        </is>
+      </c>
+      <c r="L11" s="54" t="inlineStr">
+        <is>
+          <t>Vr  KW</t>
+        </is>
+      </c>
+      <c r="M11" s="54" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="N11" s="54" t="inlineStr">
+        <is>
+          <t>ALUMBRADO</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="12" s="32">
+      <c r="B12" s="56" t="n"/>
+      <c r="C12" s="57" t="n"/>
+      <c r="D12" s="57" t="n"/>
+      <c r="E12" s="57" t="n"/>
+      <c r="F12" s="57" t="n"/>
+      <c r="G12" s="57" t="n"/>
+      <c r="H12" s="57" t="n"/>
+      <c r="I12" s="57" t="n"/>
+      <c r="J12" s="57" t="n"/>
+      <c r="K12" s="57" t="n"/>
+      <c r="L12" s="57" t="n"/>
+      <c r="M12" s="57" t="n"/>
+      <c r="N12" s="58" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="13" s="32">
+      <c r="B13" s="59" t="n"/>
+      <c r="N13" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="14" s="32">
+      <c r="B14" s="59" t="n"/>
+      <c r="N14" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" s="32">
+      <c r="B15" s="59" t="n"/>
+      <c r="N15" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="16" s="32">
+      <c r="B16" s="59" t="n"/>
+      <c r="N16" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="17" s="32">
+      <c r="B17" s="59" t="n"/>
+      <c r="N17" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="18" s="32">
+      <c r="B18" s="59" t="n"/>
+      <c r="N18" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" s="32">
+      <c r="B19" s="59" t="n"/>
+      <c r="N19" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="20" s="32">
+      <c r="B20" s="59" t="n"/>
+      <c r="N20" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="21" s="32">
+      <c r="B21" s="59" t="n"/>
+      <c r="N21" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="22" s="32">
+      <c r="B22" s="59" t="n"/>
+      <c r="N22" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="23" s="32">
+      <c r="B23" s="59" t="n"/>
+      <c r="N23" s="60" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="24" s="32">
+      <c r="B24" s="61" t="n"/>
+      <c r="C24" s="62" t="n"/>
+      <c r="D24" s="62" t="n"/>
+      <c r="E24" s="62" t="n"/>
+      <c r="F24" s="62" t="n"/>
+      <c r="G24" s="62" t="n"/>
+      <c r="H24" s="62" t="n"/>
+      <c r="I24" s="62" t="n"/>
+      <c r="J24" s="62" t="n"/>
+      <c r="K24" s="62" t="n"/>
+      <c r="L24" s="62" t="n"/>
+      <c r="M24" s="62" t="n"/>
+      <c r="N24" s="63" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="25" s="32"/>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="B9:N9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="I10:N10"/>
+  </mergeCells>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="B2:O24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.18359375" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="31" width="2.57"/>
+    <col customWidth="1" max="2" min="2" style="31" width="12.14"/>
+    <col customWidth="1" max="3" min="3" style="31" width="12.71"/>
+    <col customWidth="1" max="4" min="4" style="31" width="14.15"/>
+    <col customWidth="1" max="5" min="5" style="31" width="13.57"/>
+    <col customWidth="1" max="6" min="6" style="31" width="13.43"/>
+    <col customWidth="1" max="7" min="7" style="31" width="13.29"/>
+    <col customWidth="1" max="8" min="8" style="31" width="13.02"/>
+    <col customWidth="1" max="10" min="9" style="31" width="15.29"/>
+    <col customWidth="1" max="11" min="11" style="31" width="14.28"/>
+    <col customWidth="1" max="12" min="12" style="31" width="15.29"/>
+    <col customWidth="1" max="13" min="13" style="31" width="13.7"/>
+    <col customWidth="1" max="14" min="14" style="31" width="14.15"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15.75" r="1" s="32"/>
+    <row customHeight="1" ht="19.5" r="2" s="32">
+      <c r="B2" s="33" t="inlineStr">
+        <is>
+          <t>SERVICIO</t>
+        </is>
+      </c>
+      <c r="C2" s="34" t="n"/>
+      <c r="D2" s="35" t="inlineStr">
+        <is>
+          <t>EMPRESA</t>
+        </is>
+      </c>
+      <c r="E2" s="34" t="n"/>
+      <c r="F2" s="34" t="n"/>
+      <c r="G2" s="35" t="inlineStr">
+        <is>
+          <t>NIT</t>
+        </is>
+      </c>
+      <c r="H2" s="34" t="n"/>
+      <c r="I2" s="36" t="inlineStr">
+        <is>
+          <t>MEDIDOR</t>
+        </is>
+      </c>
+      <c r="J2" s="37" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="K2" s="34" t="n"/>
+      <c r="L2" s="34" t="n"/>
+      <c r="M2" s="34" t="n"/>
+      <c r="N2" s="38" t="n"/>
+      <c r="O2" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="3" s="32">
+      <c r="B3" s="40" t="inlineStr">
+        <is>
+          <t>ENERGIA</t>
+        </is>
+      </c>
+      <c r="C3" s="34" t="n"/>
+      <c r="D3" s="41" t="inlineStr">
+        <is>
+          <t>ELECTRICARIBE</t>
+        </is>
+      </c>
+      <c r="E3" s="34" t="n"/>
+      <c r="F3" s="34" t="n"/>
+      <c r="G3" s="41" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H3" s="34" t="n"/>
+      <c r="I3" s="42" t="n">
+        <v>25782236</v>
+      </c>
+      <c r="J3" s="43" t="inlineStr">
+        <is>
+          <t>CC. PLAZA BOCAGRANDE LOCAL 3-11</t>
+        </is>
+      </c>
+      <c r="K3" s="34" t="n"/>
+      <c r="L3" s="34" t="n"/>
+      <c r="M3" s="34" t="n"/>
+      <c r="N3" s="38" t="n"/>
+      <c r="O3" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" s="32">
+      <c r="B4" s="40" t="n"/>
+      <c r="C4" s="34" t="n"/>
+      <c r="D4" s="40" t="n"/>
+      <c r="E4" s="34" t="n"/>
+      <c r="F4" s="34" t="n"/>
+      <c r="G4" s="40" t="inlineStr">
+        <is>
+          <t>802007670/911</t>
+        </is>
+      </c>
+      <c r="H4" s="34" t="n"/>
+      <c r="I4" s="44" t="n">
+        <v>25942309</v>
+      </c>
+      <c r="J4" s="43" t="inlineStr">
+        <is>
+          <t>CR 1 12-120 ENTR BG1 LOC 311</t>
+        </is>
+      </c>
+      <c r="K4" s="34" t="n"/>
+      <c r="L4" s="34" t="n"/>
+      <c r="M4" s="34" t="n"/>
+      <c r="N4" s="38" t="n"/>
+      <c r="O4" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" s="32">
+      <c r="B5" s="45" t="n"/>
+      <c r="C5" s="34" t="n"/>
+      <c r="D5" s="40" t="inlineStr">
+        <is>
+          <t>PLAZA BOCAGRANDE CENTRO COMERCIAL</t>
+        </is>
+      </c>
+      <c r="E5" s="34" t="n"/>
+      <c r="F5" s="34" t="n"/>
+      <c r="G5" s="40" t="inlineStr">
+        <is>
+          <t>900785012/911</t>
+        </is>
+      </c>
+      <c r="H5" s="34" t="n"/>
+      <c r="I5" s="46" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J5" s="47" t="n"/>
+      <c r="K5" s="34" t="n"/>
+      <c r="L5" s="34" t="n"/>
+      <c r="M5" s="34" t="n"/>
+      <c r="N5" s="38" t="n"/>
+      <c r="O5" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" s="32">
+      <c r="B6" s="45" t="n"/>
+      <c r="C6" s="34" t="n"/>
+      <c r="D6" s="45" t="n"/>
+      <c r="E6" s="34" t="n"/>
+      <c r="F6" s="34" t="n"/>
+      <c r="G6" s="41" t="inlineStr">
+        <is>
+          <t>DEPOSITO 2 Y 4</t>
+        </is>
+      </c>
+      <c r="H6" s="34" t="n"/>
+      <c r="I6" s="48" t="n"/>
+      <c r="J6" s="47" t="n"/>
+      <c r="K6" s="34" t="n"/>
+      <c r="L6" s="34" t="n"/>
+      <c r="M6" s="34" t="n"/>
+      <c r="N6" s="38" t="n"/>
+      <c r="O6" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="32">
+      <c r="B7" s="45" t="n"/>
+      <c r="C7" s="34" t="n"/>
+      <c r="D7" s="49" t="inlineStr">
+        <is>
+          <t>CARIBERMAR DEL CARIBE</t>
+        </is>
+      </c>
+      <c r="E7" s="34" t="n"/>
+      <c r="F7" s="34" t="n"/>
+      <c r="G7" s="49" t="inlineStr">
+        <is>
+          <t>901380949/911</t>
+        </is>
+      </c>
+      <c r="H7" s="34" t="n"/>
+      <c r="I7" s="48" t="inlineStr">
+        <is>
+          <t>NIC 7742846</t>
+        </is>
+      </c>
+      <c r="J7" s="43" t="n"/>
+      <c r="K7" s="34" t="n"/>
+      <c r="L7" s="34" t="n"/>
+      <c r="M7" s="34" t="n"/>
+      <c r="N7" s="38" t="n"/>
+      <c r="O7" s="39" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="8" s="32">
+      <c r="B8" s="50" t="n"/>
+      <c r="C8" s="50" t="n"/>
+      <c r="D8" s="51" t="n"/>
+      <c r="E8" s="50" t="n"/>
+      <c r="F8" s="50" t="n"/>
+      <c r="G8" s="50" t="n"/>
+      <c r="H8" s="51" t="n"/>
+      <c r="I8" s="50" t="n"/>
+      <c r="J8" s="51" t="n"/>
+      <c r="K8" s="51" t="n"/>
+      <c r="L8" s="50" t="n"/>
+      <c r="M8" s="52" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="9" s="32">
+      <c r="B9" s="53" t="inlineStr">
+        <is>
+          <t>ENERGIA ELECTRICA</t>
+        </is>
+      </c>
+      <c r="C9" s="34" t="n"/>
+      <c r="D9" s="34" t="n"/>
+      <c r="E9" s="34" t="n"/>
+      <c r="F9" s="34" t="n"/>
+      <c r="G9" s="34" t="n"/>
+      <c r="H9" s="34" t="n"/>
+      <c r="I9" s="34" t="n"/>
+      <c r="J9" s="34" t="n"/>
+      <c r="K9" s="34" t="n"/>
+      <c r="L9" s="34" t="n"/>
+      <c r="M9" s="34" t="n"/>
+      <c r="N9" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" s="32">
+      <c r="B10" s="54" t="inlineStr">
+        <is>
+          <t>PER.DE COBRO</t>
+        </is>
+      </c>
+      <c r="C10" s="38" t="n"/>
+      <c r="D10" s="54" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="E10" s="34" t="n"/>
+      <c r="F10" s="34" t="n"/>
+      <c r="G10" s="34" t="n"/>
+      <c r="H10" s="38" t="n"/>
+      <c r="I10" s="55" t="inlineStr">
+        <is>
+          <t>INFORMACIÓN PPTOS</t>
+        </is>
+      </c>
+      <c r="J10" s="34" t="n"/>
+      <c r="K10" s="34" t="n"/>
+      <c r="L10" s="34" t="n"/>
+      <c r="M10" s="34" t="n"/>
+      <c r="N10" s="38" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="11" s="32">
+      <c r="B11" s="54" t="inlineStr">
+        <is>
+          <t>INICIAL</t>
+        </is>
+      </c>
+      <c r="C11" s="54" t="inlineStr">
+        <is>
+          <t>FINAL</t>
+        </is>
+      </c>
+      <c r="D11" s="54" t="inlineStr">
+        <is>
+          <t>CAUSA</t>
+        </is>
+      </c>
+      <c r="E11" s="54" t="inlineStr">
+        <is>
+          <t>PAGA</t>
+        </is>
+      </c>
+      <c r="F11" s="54" t="inlineStr">
+        <is>
+          <t>AJUS</t>
+        </is>
+      </c>
+      <c r="G11" s="54" t="inlineStr">
+        <is>
+          <t>DOC PAG</t>
+        </is>
+      </c>
+      <c r="H11" s="54" t="inlineStr">
+        <is>
+          <t>DOC AJ</t>
+        </is>
+      </c>
+      <c r="I11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU ACT</t>
+        </is>
+      </c>
+      <c r="J11" s="54" t="inlineStr">
+        <is>
+          <t>CONSU REAC</t>
+        </is>
+      </c>
+      <c r="K11" s="54" t="inlineStr">
+        <is>
+          <t>KW</t>
+        </is>
+      </c>
+      <c r="L11" s="54" t="inlineStr">
+        <is>
+          <t>Vr  KW</t>
+        </is>
+      </c>
+      <c r="M11" s="54" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="N11" s="54" t="inlineStr">
+        <is>
+          <t>ALUMBRADO</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="12" s="32">
+      <c r="B12" s="56" t="inlineStr">
+        <is>
+          <t>2020-09-17</t>
+        </is>
+      </c>
+      <c r="C12" s="57" t="inlineStr">
+        <is>
+          <t>2020-10-16</t>
+        </is>
+      </c>
+      <c r="D12" s="57" t="n">
+        <v>12333444</v>
+      </c>
+      <c r="E12" s="57" t="n">
+        <v>859296</v>
+      </c>
+      <c r="F12" s="57" t="n">
+        <v>-11474148</v>
+      </c>
+      <c r="G12" s="57" t="n">
+        <v>13</v>
+      </c>
+      <c r="H12" s="57" t="n">
+        <v>13</v>
+      </c>
+      <c r="I12" s="57" t="n">
+        <v>762761</v>
       </c>
       <c r="J12" s="57" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="57" t="n">
-        <v>8040</v>
+        <v>1265</v>
       </c>
       <c r="L12" s="57" t="n">
-        <v>563.5295</v>
+        <v>602.9728</v>
       </c>
       <c r="M12" s="57" t="n">
-        <v>906155</v>
+        <v>152552</v>
       </c>
       <c r="N12" s="58" t="n">
-        <v>197790</v>
+        <v>24870</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="13" s="32">
-      <c r="B13" s="59" t="inlineStr">
-        <is>
-          <t>2020-09-11</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2020-10-10</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>12000000</v>
-      </c>
-      <c r="E13" t="n">
-        <v>4760727</v>
-      </c>
-      <c r="F13" t="n">
-        <v>-7239273</v>
-      </c>
-      <c r="G13" t="n">
-        <v>45</v>
-      </c>
-      <c r="H13" t="n">
-        <v>45</v>
-      </c>
-      <c r="I13" t="n">
-        <v>4530777</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>8040</v>
-      </c>
-      <c r="L13" t="n">
-        <v>563.5295</v>
-      </c>
-      <c r="M13" t="n">
-        <v>906155</v>
-      </c>
-      <c r="N13" s="60" t="n">
-        <v>197790</v>
-      </c>
+      <c r="B13" s="59" t="n"/>
+      <c r="N13" s="60" t="n"/>
     </row>
     <row customHeight="1" ht="15.75" r="14" s="32">
       <c r="B14" s="59" t="n"/>

</xml_diff>

<commit_message>
error con la consulta del mes
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -1532,91 +1532,91 @@
     <row customHeight="1" ht="15.75" r="12" s="32">
       <c r="B12" s="56" t="inlineStr">
         <is>
-          <t>2020-09-06</t>
+          <t>2020-02-03</t>
         </is>
       </c>
       <c r="C12" s="57" t="inlineStr">
         <is>
-          <t>2020-10-06</t>
+          <t>2020-03-04</t>
         </is>
       </c>
       <c r="D12" s="57" t="n">
-        <v>12333333</v>
+        <v>1233333</v>
       </c>
       <c r="E12" s="57" t="n">
-        <v>1491386</v>
+        <v>42549</v>
       </c>
       <c r="F12" s="57" t="n">
-        <v>-10841947</v>
+        <v>-1190784</v>
       </c>
       <c r="G12" s="57" t="n">
-        <v>122</v>
+        <v>12</v>
       </c>
       <c r="H12" s="57" t="n">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="I12" s="57" t="n">
-        <v>1284935</v>
+        <v>41916</v>
       </c>
       <c r="J12" s="57" t="n">
-        <v>80026</v>
+        <v>0</v>
       </c>
       <c r="K12" s="57" t="n">
-        <v>2131</v>
+        <v>70</v>
       </c>
       <c r="L12" s="57" t="n">
-        <v>602.9728</v>
+        <v>598.7989</v>
       </c>
       <c r="M12" s="57" t="n">
-        <v>256987</v>
+        <v>0</v>
       </c>
       <c r="N12" s="58" t="n">
-        <v>58680</v>
+        <v>7020</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="13" s="32">
       <c r="B13" s="59" t="inlineStr">
         <is>
-          <t>2020-09-11</t>
+          <t>2020-05-05</t>
         </is>
       </c>
       <c r="C13" s="31" t="inlineStr">
         <is>
-          <t>2020-10-10</t>
+          <t>2020-06-03</t>
         </is>
       </c>
       <c r="D13" s="31" t="n">
-        <v>12000000</v>
+        <v>1333333</v>
       </c>
       <c r="E13" s="31" t="n">
-        <v>4760727</v>
+        <v>13579</v>
       </c>
       <c r="F13" s="31" t="n">
-        <v>-7239273</v>
+        <v>-1319754</v>
       </c>
       <c r="G13" s="31" t="n">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="H13" s="31" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="I13" s="31" t="n">
-        <v>4530777</v>
+        <v>73563</v>
       </c>
       <c r="J13" s="31" t="n">
         <v>0</v>
       </c>
       <c r="K13" s="31" t="n">
-        <v>8040</v>
+        <v>122</v>
       </c>
       <c r="L13" s="31" t="n">
-        <v>563.5295</v>
+        <v>602.9728</v>
       </c>
       <c r="M13" s="31" t="n">
-        <v>906155</v>
+        <v>0</v>
       </c>
       <c r="N13" s="60" t="n">
-        <v>197790</v>
+        <v>60</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="14" s="32">

</xml_diff>